<commit_message>
#8990 - undo soft delete for contacts
</commit_message>
<xml_diff>
--- a/sormas-api/src/main/resources/doc/SORMAS_User_Roles.xlsx
+++ b/sormas-api/src/main/resources/doc/SORMAS_User_Roles.xlsx
@@ -565,7 +565,7 @@
     <t>No</t>
   </si>
   <si>
-    <t>U747D3-NM65DB-WR7QZZ-KC2NCIZE</t>
+    <t>SVBQ4Q-M6LXCK-EILBRB-RV7RKHEQ</t>
   </si>
   <si>
     <t>Admin Surveillance Supervisor</t>
@@ -574,13 +574,13 @@
     <t>Region</t>
   </si>
   <si>
-    <t>VDFMCV-YTRS6Q-XEINFL-QJOVCC6U</t>
+    <t>T2YFVQ-UALTV7-C6FPVV-5XUUSBAQ</t>
   </si>
   <si>
     <t>BAG User</t>
   </si>
   <si>
-    <t>XQIVZG-D6TK3D-JD6QYU-BUY7KIYA</t>
+    <t>WXUVOC-2FEOLI-MBR6FK-R2PO2KM4</t>
   </si>
   <si>
     <t>Case Officer</t>
@@ -589,13 +589,13 @@
     <t>District</t>
   </si>
   <si>
-    <t>WV3LXO-56LNGV-3IZBUP-GIOR2GFE</t>
+    <t>TD5YWN-CTNFSD-OXU5UQ-P7T72BOM</t>
   </si>
   <si>
     <t>Clinician</t>
   </si>
   <si>
-    <t>UZYLRH-EFDUOX-KUJ3EG-DUWK2DY4</t>
+    <t>UYDITU-7Q6BHJ-7UB4GK-WXEUSCIE</t>
   </si>
   <si>
     <t>Community Informant</t>
@@ -604,37 +604,37 @@
     <t>Community</t>
   </si>
   <si>
-    <t>XYAEFU-HYAXDI-725ONV-7TEFSBFU</t>
+    <t>TSNCUO-G52ZP2-A7N5T2-M4J2KBAE</t>
   </si>
   <si>
     <t>Community Officer</t>
   </si>
   <si>
-    <t>T7NTCD-DEKMW5-S6AD5M-4NBIKJO4</t>
+    <t>QALKMH-U23NN7-WTJA7L-73E2CHKM</t>
   </si>
   <si>
     <t>Contact Officer</t>
   </si>
   <si>
-    <t>RCMKDX-EQLAE2-NHD3BC-BR3M2OZU</t>
+    <t>XNR6EZ-KJDB7Y-LI57LH-4VF42I2Y</t>
   </si>
   <si>
     <t>Contact Supervisor</t>
   </si>
   <si>
-    <t>WYQ2RB-YA2ELL-K7KJHK-5EZHCBYY</t>
+    <t>SZ3DX5-4AGEJE-ZGPSYH-SVNFCFM4</t>
   </si>
   <si>
     <t>District Observer</t>
   </si>
   <si>
-    <t>SBC4W3-FLYTHP-6VTPSH-XMUNCDYU</t>
+    <t>V27GIG-USYWMJ-G2JPTP-4SHJCBY4</t>
   </si>
   <si>
     <t>Event Officer</t>
   </si>
   <si>
-    <t>XWO2OV-PHYVTN-ONJONK-CTAL2N4A</t>
+    <t>WWCW3B-A6E6X4-3JZ4YF-P5AKKKVI</t>
   </si>
   <si>
     <t>External Lab Officer</t>
@@ -643,7 +643,7 @@
     <t>External laboratory</t>
   </si>
   <si>
-    <t>WI4WZ3-ESGPVY-K5LU3T-DVXWKNUE</t>
+    <t>TKDQAO-JJGR7Q-XJAV7V-V2RKCORE</t>
   </si>
   <si>
     <t>External Visits User</t>
@@ -652,7 +652,7 @@
     <t>Nation</t>
   </si>
   <si>
-    <t>UYWCH4-FJAGER-2ACPVM-IJPMSLIA</t>
+    <t>QMRO57-QLHTNI-RI6J3T-6L4Q2PAM</t>
   </si>
   <si>
     <t>Hospital Informant</t>
@@ -661,13 +661,13 @@
     <t>Facility</t>
   </si>
   <si>
-    <t>TVM3BX-TNWMTL-IOKHA3-HIDMSNWM</t>
+    <t>VN7AL2-XTVNCR-DNHKZD-SG2NKCAQ</t>
   </si>
   <si>
     <t>Import User</t>
   </si>
   <si>
-    <t>Q7XTYT-NXGRV7-MZCM72-PJI6SJNI</t>
+    <t>T4N6N4-U63KOE-MID5YP-LNO6CNV4</t>
   </si>
   <si>
     <t>Lab Officer</t>
@@ -676,25 +676,25 @@
     <t>Laboratory</t>
   </si>
   <si>
-    <t>XM2CKA-JH4XLH-ITNFMA-PMEUCKE4</t>
+    <t>SAPEKQ-BKXSWW-WGC4DO-N4YTSOXA</t>
   </si>
   <si>
     <t>National Clinician</t>
   </si>
   <si>
-    <t>VTYTZS-YIZJGZ-XDCZUX-6LASKP5E</t>
+    <t>TA6WR3-PDRG4C-YQGWXI-I4CISIAI</t>
   </si>
   <si>
     <t>National Observer</t>
   </si>
   <si>
-    <t>VRCKMH-VZ4PCU-RLIGJK-VTT6SKBM</t>
+    <t>XL3EZD-QZMGLW-H5RC3V-DN3BCGDE</t>
   </si>
   <si>
     <t>National User</t>
   </si>
   <si>
-    <t>THVPON-N2KIAV-HVW3HB-4YQC2CT4</t>
+    <t>WA7ZUG-HOILVH-TBPP7C-XSRQSCRQ</t>
   </si>
   <si>
     <t>POE Informant</t>
@@ -703,43 +703,43 @@
     <t>Point of entry</t>
   </si>
   <si>
-    <t>XF4CRI-ZFPMYE-ZYF6GK-JESZCD6U</t>
+    <t>TRBFTM-MGJ2EP-OOSZG4-B3J7KJDE</t>
   </si>
   <si>
     <t>POE National User</t>
   </si>
   <si>
-    <t>RQKG7J-AT6NDJ-3BMVD5-FTK22LDI</t>
+    <t>UYIJ57-TIVXP3-GZUGCT-TIOM2PDU</t>
   </si>
   <si>
     <t>POE Supervisor</t>
   </si>
   <si>
-    <t>T44AYC-UIT3W5-42JHEK-TJOHKE5M</t>
+    <t>RVZ4CV-MTFUKQ-C6A5HV-IJHZCIGM</t>
   </si>
   <si>
     <t>Region Observer</t>
   </si>
   <si>
-    <t>V34LKQ-Q65T6Y-AALGOD-XIYNSDQI</t>
+    <t>VWIIWC-6YFPZI-HLP4PW-C7MMCEFY</t>
   </si>
   <si>
     <t>Sormas to Sormas Client</t>
   </si>
   <si>
-    <t>UHCKZK-O4OOBH-VRJQ35-JP44KK7M</t>
+    <t>RTO2PS-2MTJJH-RMBU4T-FUYUKBHA</t>
   </si>
   <si>
     <t>Surveillance Officer</t>
   </si>
   <si>
-    <t>XSQHXN-P4WH74-VUDC4F-LPIISCYY</t>
+    <t>RENBVH-NKED45-67G6VS-FB5QCDB4</t>
   </si>
   <si>
     <t>Surveillance Supervisor</t>
   </si>
   <si>
-    <t>SQWC5Y-UHX7B6-RC2Z5W-M3U2KD6E</t>
+    <t>UVM2VS-WYGJMH-VW3KPF-XJUE2FWQ</t>
   </si>
   <si>
     <t>User Right</t>
@@ -778,7 +778,7 @@
     <t>Able to edit existing cases</t>
   </si>
   <si>
-    <t>PERSON_VIEW, PERSON_EDIT, CASE_VIEW</t>
+    <t>PERSON_EDIT, PERSON_VIEW, CASE_VIEW</t>
   </si>
   <si>
     <t>Archive cases</t>
@@ -793,7 +793,7 @@
     <t>Able to delete cases from the system</t>
   </si>
   <si>
-    <t>DOCUMENT_VIEW, ADDITIONAL_TEST_VIEW, PERSON_DELETE, TASK_VIEW, SAMPLE_DELETE, TREATMENT_DELETE, THERAPY_VIEW, ADDITIONAL_TEST_DELETE, PRESCRIPTION_DELETE, CLINICAL_COURSE_VIEW, VISIT_DELETE, CLINICAL_VISIT_DELETE, IMMUNIZATION_DELETE, PATHOGEN_TEST_DELETE, DOCUMENT_DELETE, PERSON_VIEW, SAMPLE_VIEW, TASK_DELETE, IMMUNIZATION_VIEW, CASE_VIEW</t>
+    <t>DOCUMENT_VIEW, VISIT_DELETE, TASK_DELETE, IMMUNIZATION_DELETE, TREATMENT_DELETE, PATHOGEN_TEST_DELETE, CLINICAL_COURSE_VIEW, CLINICAL_VISIT_DELETE, PERSON_VIEW, SAMPLE_DELETE, ADDITIONAL_TEST_DELETE, PERSON_DELETE, TASK_VIEW, IMMUNIZATION_VIEW, PRESCRIPTION_DELETE, THERAPY_VIEW, DOCUMENT_DELETE, CASE_VIEW, SAMPLE_VIEW, ADDITIONAL_TEST_VIEW</t>
   </si>
   <si>
     <t>Import cases into SORMAS</t>
@@ -814,7 +814,7 @@
     <t>Able to edit case investigation status</t>
   </si>
   <si>
-    <t>CASE_EDIT, PERSON_VIEW, PERSON_EDIT, CASE_VIEW</t>
+    <t>CASE_EDIT, PERSON_EDIT, PERSON_VIEW, CASE_VIEW</t>
   </si>
   <si>
     <t>Edit case classification and outcome</t>
@@ -877,7 +877,7 @@
     <t>Able to create new immunizations and vaccinations</t>
   </si>
   <si>
-    <t>PERSON_VIEW, IMMUNIZATION_VIEW</t>
+    <t>IMMUNIZATION_VIEW, PERSON_VIEW</t>
   </si>
   <si>
     <t>Edit existing immunizations and vaccinations</t>
@@ -886,7 +886,7 @@
     <t>Able to edit existing immunizations and vaccinations</t>
   </si>
   <si>
-    <t>PERSON_VIEW, IMMUNIZATION_VIEW, PERSON_EDIT</t>
+    <t>PERSON_EDIT, IMMUNIZATION_VIEW, PERSON_VIEW</t>
   </si>
   <si>
     <t>Archive immunizations</t>
@@ -901,7 +901,7 @@
     <t>Able to delete immunizations and vaccinations from the system</t>
   </si>
   <si>
-    <t>PERSON_DELETE, PERSON_VIEW, IMMUNIZATION_VIEW, VISIT_DELETE</t>
+    <t>PERSON_DELETE, IMMUNIZATION_VIEW, VISIT_DELETE, PERSON_VIEW</t>
   </si>
   <si>
     <t>Persons</t>
@@ -928,7 +928,7 @@
     <t>Able to delete persons from the system</t>
   </si>
   <si>
-    <t>PERSON_VIEW, VISIT_DELETE</t>
+    <t>VISIT_DELETE, PERSON_VIEW</t>
   </si>
   <si>
     <t>Export persons</t>
@@ -943,7 +943,7 @@
     <t>Able to delete person contact details</t>
   </si>
   <si>
-    <t>PERSON_VIEW, PERSON_EDIT</t>
+    <t>PERSON_EDIT, PERSON_VIEW</t>
   </si>
   <si>
     <t>Sample Testing</t>
@@ -973,7 +973,7 @@
     <t>Able to delete samples from the system</t>
   </si>
   <si>
-    <t>PATHOGEN_TEST_DELETE, ADDITIONAL_TEST_VIEW, SAMPLE_VIEW, ADDITIONAL_TEST_DELETE</t>
+    <t>ADDITIONAL_TEST_DELETE, PATHOGEN_TEST_DELETE, SAMPLE_VIEW, ADDITIONAL_TEST_VIEW</t>
   </si>
   <si>
     <t>Export samples from SORMAS</t>
@@ -1033,7 +1033,7 @@
     <t>Able to create new additional tests</t>
   </si>
   <si>
-    <t>ADDITIONAL_TEST_VIEW, SAMPLE_VIEW</t>
+    <t>SAMPLE_VIEW, ADDITIONAL_TEST_VIEW</t>
   </si>
   <si>
     <t>Edit existing additional tests</t>
@@ -1063,7 +1063,7 @@
     <t>Able to create new contacts</t>
   </si>
   <si>
-    <t>PERSON_VIEW, CONTACT_VIEW, CASE_VIEW</t>
+    <t>CONTACT_VIEW, PERSON_VIEW, CASE_VIEW</t>
   </si>
   <si>
     <t>Edit existing contacts</t>
@@ -1072,7 +1072,7 @@
     <t>Able to edit existing contacts</t>
   </si>
   <si>
-    <t>PERSON_VIEW, CONTACT_VIEW, PERSON_EDIT, CASE_VIEW</t>
+    <t>PERSON_EDIT, CONTACT_VIEW, PERSON_VIEW, CASE_VIEW</t>
   </si>
   <si>
     <t>Archive contacts</t>
@@ -1087,7 +1087,7 @@
     <t>Able to delete contacts from the system</t>
   </si>
   <si>
-    <t>DOCUMENT_VIEW, ADDITIONAL_TEST_VIEW, PERSON_DELETE, TASK_VIEW, SAMPLE_DELETE, CONTACT_VIEW, ADDITIONAL_TEST_DELETE, VISIT_DELETE, PATHOGEN_TEST_DELETE, DOCUMENT_DELETE, PERSON_VIEW, SAMPLE_VIEW, TASK_DELETE, CASE_VIEW</t>
+    <t>DOCUMENT_VIEW, VISIT_DELETE, TASK_DELETE, PATHOGEN_TEST_DELETE, PERSON_VIEW, SAMPLE_DELETE, ADDITIONAL_TEST_DELETE, PERSON_DELETE, TASK_VIEW, CONTACT_VIEW, DOCUMENT_DELETE, SAMPLE_VIEW, CASE_VIEW, ADDITIONAL_TEST_VIEW</t>
   </si>
   <si>
     <t>Import contacts</t>
@@ -1108,7 +1108,7 @@
     <t>Able to create resulting cases from contacts</t>
   </si>
   <si>
-    <t>CASE_CREATE, PERSON_VIEW, CONTACT_VIEW, PERSON_EDIT, CONTACT_EDIT, CASE_VIEW</t>
+    <t>PERSON_EDIT, CONTACT_EDIT, CONTACT_VIEW, PERSON_VIEW, CASE_CREATE, CASE_VIEW</t>
   </si>
   <si>
     <t>Reassign the source case of contacts</t>
@@ -1117,7 +1117,7 @@
     <t>Able to reassign the source case of contacts</t>
   </si>
   <si>
-    <t>PERSON_VIEW, CONTACT_VIEW, PERSON_EDIT, CONTACT_EDIT, CASE_VIEW</t>
+    <t>PERSON_EDIT, CONTACT_EDIT, CONTACT_VIEW, PERSON_VIEW, CASE_VIEW</t>
   </si>
   <si>
     <t>Merge contacts</t>
@@ -1195,7 +1195,7 @@
     <t>Able to assign tasks to users</t>
   </si>
   <si>
-    <t>TASK_VIEW, TASK_EDIT</t>
+    <t>TASK_EDIT, TASK_VIEW</t>
   </si>
   <si>
     <t>Events</t>
@@ -1213,7 +1213,7 @@
     <t>Able to delete actions from the system</t>
   </si>
   <si>
-    <t>DOCUMENT_VIEW, DOCUMENT_DELETE, EVENT_VIEW</t>
+    <t>EVENT_VIEW, DOCUMENT_VIEW, DOCUMENT_DELETE</t>
   </si>
   <si>
     <t>Edit existing actions</t>
@@ -1252,7 +1252,7 @@
     <t>Able to delete events from the system</t>
   </si>
   <si>
-    <t>DOCUMENT_VIEW, ADDITIONAL_TEST_VIEW, TASK_VIEW, PERSON_DELETE, SAMPLE_DELETE, ADDITIONAL_TEST_DELETE, VISIT_DELETE, EVENTPARTICIPANT_VIEW, PATHOGEN_TEST_DELETE, DOCUMENT_DELETE, PERSON_VIEW, SAMPLE_VIEW, TASK_DELETE, ACTION_DELETE, EVENT_VIEW, EVENTPARTICIPANT_DELETE</t>
+    <t>DOCUMENT_VIEW, ACTION_DELETE, VISIT_DELETE, TASK_DELETE, PATHOGEN_TEST_DELETE, PERSON_VIEW, SAMPLE_DELETE, ADDITIONAL_TEST_DELETE, EVENT_VIEW, EVENTPARTICIPANT_DELETE, PERSON_DELETE, TASK_VIEW, DOCUMENT_DELETE, EVENTPARTICIPANT_VIEW, SAMPLE_VIEW, ADDITIONAL_TEST_VIEW</t>
   </si>
   <si>
     <t>Import events</t>
@@ -1273,7 +1273,7 @@
     <t>Able to perform bulk operations in the event directory</t>
   </si>
   <si>
-    <t>EVENT_EDIT, EVENT_VIEW</t>
+    <t>EVENT_VIEW, EVENT_EDIT</t>
   </si>
   <si>
     <t>Can be responsible for an event</t>
@@ -1285,7 +1285,7 @@
     <t>Able to view existing event participants</t>
   </si>
   <si>
-    <t>PERSON_VIEW, EVENT_VIEW</t>
+    <t>EVENT_VIEW, PERSON_VIEW</t>
   </si>
   <si>
     <t>Create new event participants</t>
@@ -1294,7 +1294,7 @@
     <t>Able to create new event participants</t>
   </si>
   <si>
-    <t>EVENTPARTICIPANT_VIEW, PERSON_VIEW, EVENT_VIEW</t>
+    <t>EVENT_VIEW, PERSON_VIEW, EVENTPARTICIPANT_VIEW</t>
   </si>
   <si>
     <t>Edit existing event participants</t>
@@ -1303,7 +1303,7 @@
     <t>Able to edit existing event participants</t>
   </si>
   <si>
-    <t>EVENTPARTICIPANT_VIEW, PERSON_VIEW, PERSON_EDIT, EVENT_VIEW</t>
+    <t>EVENT_VIEW, PERSON_EDIT, PERSON_VIEW, EVENTPARTICIPANT_VIEW</t>
   </si>
   <si>
     <t>Event participant archive</t>
@@ -1318,7 +1318,7 @@
     <t>Able to delete event participants from the system</t>
   </si>
   <si>
-    <t>EVENTPARTICIPANT_VIEW, PATHOGEN_TEST_DELETE, ADDITIONAL_TEST_VIEW, PERSON_DELETE, SAMPLE_DELETE, PERSON_VIEW, SAMPLE_VIEW, ADDITIONAL_TEST_DELETE, EVENT_VIEW, VISIT_DELETE</t>
+    <t>SAMPLE_DELETE, ADDITIONAL_TEST_DELETE, EVENT_VIEW, PERSON_DELETE, VISIT_DELETE, PATHOGEN_TEST_DELETE, PERSON_VIEW, EVENTPARTICIPANT_VIEW, SAMPLE_VIEW, ADDITIONAL_TEST_VIEW</t>
   </si>
   <si>
     <t>Import event participants</t>
@@ -1333,7 +1333,7 @@
     <t>Able to perform bulk operations in the event participants directory</t>
   </si>
   <si>
-    <t>EVENTPARTICIPANT_VIEW, EVENTPARTICIPANT_EDIT, PERSON_VIEW, PERSON_EDIT, EVENT_VIEW</t>
+    <t>EVENT_VIEW, PERSON_EDIT, EVENTPARTICIPANT_EDIT, PERSON_VIEW, EVENTPARTICIPANT_VIEW</t>
   </si>
   <si>
     <t>Create new event groups</t>
@@ -1477,7 +1477,7 @@
     <t>Able to view contact transmission chains on the dashboard</t>
   </si>
   <si>
-    <t>PERSON_VIEW, CONTACT_VIEW, DASHBOARD_CONTACT_VIEW, CASE_VIEW</t>
+    <t>DASHBOARD_CONTACT_VIEW, CONTACT_VIEW, PERSON_VIEW, CASE_VIEW</t>
   </si>
   <si>
     <t>Access campaigns dashboard</t>
@@ -1507,7 +1507,7 @@
     <t>Able to create new prescriptions</t>
   </si>
   <si>
-    <t>PERSON_VIEW, THERAPY_VIEW, CASE_VIEW</t>
+    <t>THERAPY_VIEW, PERSON_VIEW, CASE_VIEW</t>
   </si>
   <si>
     <t>Edit existing prescriptions</t>
@@ -1552,7 +1552,7 @@
     <t>Able to edit the clinical course of cases</t>
   </si>
   <si>
-    <t>PERSON_VIEW, THERAPY_VIEW, CLINICAL_COURSE_VIEW, CASE_VIEW</t>
+    <t>THERAPY_VIEW, CLINICAL_COURSE_VIEW, PERSON_VIEW, CASE_VIEW</t>
   </si>
   <si>
     <t>Create new clinical visits</t>
@@ -1588,7 +1588,7 @@
     <t>Able to edit existing port health info</t>
   </si>
   <si>
-    <t>PERSON_VIEW, PORT_HEALTH_INFO_VIEW, CASE_VIEW</t>
+    <t>PORT_HEALTH_INFO_VIEW, PERSON_VIEW, CASE_VIEW</t>
   </si>
   <si>
     <t>Aggregated Reporting</t>
@@ -1678,7 +1678,7 @@
     <t>Able to delete campaigns from the system</t>
   </si>
   <si>
-    <t>CAMPAIGN_VIEW, CAMPAIGN_FORM_DATA_VIEW, CAMPAIGN_FORM_DATA_DELETE</t>
+    <t>CAMPAIGN_FORM_DATA_DELETE, CAMPAIGN_FORM_DATA_VIEW, CAMPAIGN_VIEW</t>
   </si>
   <si>
     <t>View existing campaign form data</t>
@@ -1735,7 +1735,7 @@
     <t>Able to create new travel entries</t>
   </si>
   <si>
-    <t>TRAVEL_ENTRY_MANAGEMENT_ACCESS, PERSON_VIEW, TRAVEL_ENTRY_VIEW</t>
+    <t>TRAVEL_ENTRY_VIEW, TRAVEL_ENTRY_MANAGEMENT_ACCESS, PERSON_VIEW</t>
   </si>
   <si>
     <t>Edit existing travel entries</t>
@@ -1744,7 +1744,7 @@
     <t>Able to edit existing travel entries</t>
   </si>
   <si>
-    <t>TRAVEL_ENTRY_MANAGEMENT_ACCESS, PERSON_VIEW, TRAVEL_ENTRY_VIEW, PERSON_EDIT</t>
+    <t>PERSON_EDIT, TRAVEL_ENTRY_VIEW, TRAVEL_ENTRY_MANAGEMENT_ACCESS, PERSON_VIEW</t>
   </si>
   <si>
     <t>Archive travel entries</t>
@@ -1759,7 +1759,7 @@
     <t>Able to delete travel entries from the system</t>
   </si>
   <si>
-    <t>DOCUMENT_VIEW, TRAVEL_ENTRY_MANAGEMENT_ACCESS, PERSON_DELETE, TASK_VIEW, DOCUMENT_DELETE, PERSON_VIEW, TASK_DELETE, TRAVEL_ENTRY_VIEW, VISIT_DELETE</t>
+    <t>DOCUMENT_VIEW, PERSON_DELETE, TASK_VIEW, VISIT_DELETE, TRAVEL_ENTRY_VIEW, TASK_DELETE, DOCUMENT_DELETE, TRAVEL_ENTRY_MANAGEMENT_ACCESS, PERSON_VIEW</t>
   </si>
   <si>
     <t>Documents</t>
@@ -1885,7 +1885,7 @@
     <t>Able to work with messages</t>
   </si>
   <si>
-    <t>PERSON_DELETE, CASE_CREATE, EVENTPARTICIPANT_CREATE, EVENT_EDIT, CONTACT_EDIT, PATHOGEN_TEST_CREATE, EVENTPARTICIPANT_VIEW, PERSON_VIEW, IMMUNIZATION_CREATE, IMMUNIZATION_VIEW, SAMPLE_CREATE, IMMUNIZATION_EDIT, CASE_VIEW, SAMPLE_EDIT, EXTERNAL_MESSAGE_VIEW, CASE_EDIT, CONTACT_VIEW, PATHOGEN_TEST_EDIT, PERSON_EDIT, VISIT_DELETE, IMMUNIZATION_DELETE, CONTACT_CREATE, PATHOGEN_TEST_DELETE, EVENTPARTICIPANT_EDIT, EVENT_CREATE, SAMPLE_VIEW, EVENT_VIEW</t>
+    <t>IMMUNIZATION_DELETE, SAMPLE_EDIT, EVENT_VIEW, PERSON_EDIT, PERSON_DELETE, IMMUNIZATION_VIEW, CONTACT_VIEW, CASE_CREATE, EVENTPARTICIPANT_VIEW, SAMPLE_CREATE, CASE_EDIT, IMMUNIZATION_EDIT, IMMUNIZATION_CREATE, VISIT_DELETE, PATHOGEN_TEST_DELETE, EVENTPARTICIPANT_EDIT, PERSON_VIEW, PATHOGEN_TEST_CREATE, CONTACT_CREATE, CONTACT_EDIT, EVENTPARTICIPANT_CREATE, EVENT_EDIT, EVENT_CREATE, CASE_VIEW, SAMPLE_VIEW, EXTERNAL_MESSAGE_VIEW, PATHOGEN_TEST_EDIT</t>
   </si>
   <si>
     <t>Delete messages from the system</t>
@@ -1942,7 +1942,7 @@
     <t>SORMAS Version</t>
   </si>
   <si>
-    <t>1.76.0-SNAPSHOT</t>
+    <t>1.0.0</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
#10214 - set ManyToOne relations of cached entities to lazy where missing        - add cache annotation to collections of cached entities as well
</commit_message>
<xml_diff>
--- a/sormas-api/src/main/resources/doc/SORMAS_User_Roles.xlsx
+++ b/sormas-api/src/main/resources/doc/SORMAS_User_Roles.xlsx
@@ -568,7 +568,7 @@
     <t>No</t>
   </si>
   <si>
-    <t>VT4XTW-LZ6PWX-YQB3IN-PNU62EQU</t>
+    <t>QJCP7Z-AD2A2D-YJWYXL-7BLW2D3I</t>
   </si>
   <si>
     <t>Admin Surveillance Supervisor</t>
@@ -577,13 +577,13 @@
     <t>Region</t>
   </si>
   <si>
-    <t>UGQTP6-C45MRT-TQAHAH-6QYDSPWA</t>
+    <t>RSNKSP-LUEDRG-BZEH5O-KEZO2EFI</t>
   </si>
   <si>
     <t>BAG User</t>
   </si>
   <si>
-    <t>XWXPJB-QLGTWV-DET6JL-O4SQSPFQ</t>
+    <t>TBIGFY-OFUONA-UTN5OR-EQ6FCBJM</t>
   </si>
   <si>
     <t>Case Officer</t>
@@ -592,13 +592,13 @@
     <t>District</t>
   </si>
   <si>
-    <t>VXRAF2-GOEJS3-LQNNBT-BOBRKIYI</t>
+    <t>TNHILE-XKAZ5L-NSIDFH-TZ3UKIYY</t>
   </si>
   <si>
     <t>Clinician</t>
   </si>
   <si>
-    <t>SDVHV4-BDW34F-GYUP5O-233HCBVM</t>
+    <t>UTQNR6-VRTKWZ-U42SEQ-DDJZCKBI</t>
   </si>
   <si>
     <t>Community Informant</t>
@@ -607,37 +607,37 @@
     <t>Community</t>
   </si>
   <si>
-    <t>TCKL5X-XFAWDE-U2QONF-Y7XZCHRI</t>
+    <t>V52HST-R5GAPK-KUS2FB-IY2OKHFI</t>
   </si>
   <si>
     <t>Community Officer</t>
   </si>
   <si>
-    <t>X2VOQH-TXEGG5-LVQ74V-NJ4CCJFY</t>
+    <t>WDNLR4-QODXES-TA3EDM-42CM2P2Y</t>
   </si>
   <si>
     <t>Contact Officer</t>
   </si>
   <si>
-    <t>RSRBWL-C4QQQP-SZ4AIV-SC5H2DLQ</t>
+    <t>S7ANPX-YN3Q2R-MEPIQG-IWGQCOFU</t>
   </si>
   <si>
     <t>Contact Supervisor</t>
   </si>
   <si>
-    <t>QLXWLO-JUGW7G-WG3PQZ-RXFV2AJI</t>
+    <t>XTYY5L-YU3OJF-YYVEGP-AHEYKDNU</t>
   </si>
   <si>
     <t>District Observer</t>
   </si>
   <si>
-    <t>TSFVEM-5LVBIT-IH4MZD-WYU2SLJY</t>
+    <t>X7S5GU-HF3FBA-6CJ7XA-LKBD2E2A</t>
   </si>
   <si>
     <t>Event Officer</t>
   </si>
   <si>
-    <t>S2UGHM-TS2AW2-LGUEKE-SHTLKEMA</t>
+    <t>VTKRYY-XKJCZV-6UWMIJ-45ZVSA74</t>
   </si>
   <si>
     <t>External Lab Officer</t>
@@ -646,7 +646,7 @@
     <t>External laboratory</t>
   </si>
   <si>
-    <t>UKYL2M-TYOU2Z-XRWHQD-B36R2NJQ</t>
+    <t>WBZTYE-N4RVK4-XZMUFZ-NFXOSETQ</t>
   </si>
   <si>
     <t>External Visits User</t>
@@ -655,7 +655,7 @@
     <t>Nation</t>
   </si>
   <si>
-    <t>TSUNLK-DSZINO-HH7I72-6C7OCPGU</t>
+    <t>SINIIY-7EKXCP-A6R3BX-WEV52A2U</t>
   </si>
   <si>
     <t>Hospital Informant</t>
@@ -664,13 +664,13 @@
     <t>Facility</t>
   </si>
   <si>
-    <t>RGTJ53-72OAUX-GUSLVV-MVLA2NGA</t>
+    <t>QNWFWI-4CHEFD-WTOGKD-7LP3CG7M</t>
   </si>
   <si>
     <t>Import User</t>
   </si>
   <si>
-    <t>WVX4OH-ZG2KIR-KCNOIF-OBPMCEPU</t>
+    <t>RVLNRH-MU5HSI-AJZMXS-BXRB2GQI</t>
   </si>
   <si>
     <t>Lab Officer</t>
@@ -679,25 +679,25 @@
     <t>Laboratory</t>
   </si>
   <si>
-    <t>QKGYP7-OXFTNR-7XPIS6-TK4BKDXA</t>
+    <t>TA37XI-I5ITUM-ORVBNZ-76DUCHDQ</t>
   </si>
   <si>
     <t>National Clinician</t>
   </si>
   <si>
-    <t>RSFRVS-UZ3RNC-S3IGX4-TWLACHQA</t>
+    <t>QDO6BR-DUDGQ6-7CH5B6-IQ3WSIMA</t>
   </si>
   <si>
     <t>National Observer</t>
   </si>
   <si>
-    <t>QRSVG6-35ZOQZ-TUPV2X-QFPNSOEQ</t>
+    <t>XUKH5K-HL6NQH-QXCG2N-M42GKCHI</t>
   </si>
   <si>
     <t>National User</t>
   </si>
   <si>
-    <t>TFC2FN-7AHGUP-DUFNNK-JRSO2EYA</t>
+    <t>XBEFLD-IZKOTV-XB6DHT-3ZM4KINI</t>
   </si>
   <si>
     <t>POE Informant</t>
@@ -706,43 +706,43 @@
     <t>Point of entry</t>
   </si>
   <si>
-    <t>XRLFFM-7M344D-6RN6CO-KTLIKEEA</t>
+    <t>QPC4DB-ZPE6RR-CARHKB-KBKJ2MV4</t>
   </si>
   <si>
     <t>POE National User</t>
   </si>
   <si>
-    <t>RUIVAF-RJIEJI-IBUDBL-EBW4KNAI</t>
+    <t>TBSJAA-LICJEI-UK5INB-2LFECNXE</t>
   </si>
   <si>
     <t>POE Supervisor</t>
   </si>
   <si>
-    <t>W6OKBI-KAMOKQ-S7F2ML-HOSDCOQ4</t>
+    <t>UH74FA-L4N3SM-4ZISGJ-RTXN2FJ4</t>
   </si>
   <si>
     <t>Region Observer</t>
   </si>
   <si>
-    <t>X7UFJA-7JTSFL-C4AUD5-NXFC2FNI</t>
+    <t>T3SETM-J6GC4Q-VPKEBV-TEMSSFJ4</t>
   </si>
   <si>
     <t>Sormas to Sormas Client</t>
   </si>
   <si>
-    <t>ROQFF4-5EUQNC-3EQPDF-GPHLSPHY</t>
+    <t>WRPTSW-SMWVNR-4EOG3X-JY7W2JU4</t>
   </si>
   <si>
     <t>Surveillance Officer</t>
   </si>
   <si>
-    <t>VEFHK5-GSHAH2-XCE7UP-RC5I2NOE</t>
+    <t>U3INAZ-FOAO5T-TDFBVH-MFVAKFLU</t>
   </si>
   <si>
     <t>Surveillance Supervisor</t>
   </si>
   <si>
-    <t>U3KEOR-OCPH5D-6E72OK-UCU62DJU</t>
+    <t>QYFL24-R2JSCQ-PHLA4I-MQL2CLSE</t>
   </si>
   <si>
     <t>User Right</t>
@@ -781,7 +781,7 @@
     <t>Able to edit existing cases</t>
   </si>
   <si>
-    <t>PERSON_EDIT, PERSON_VIEW, CASE_VIEW</t>
+    <t>PERSON_VIEW, PERSON_EDIT, CASE_VIEW</t>
   </si>
   <si>
     <t>Archive cases</t>
@@ -796,7 +796,7 @@
     <t>Able to delete cases from the system</t>
   </si>
   <si>
-    <t>SAMPLE_DELETE, PATHOGEN_TEST_DELETE, DOCUMENT_VIEW, THERAPY_VIEW, CLINICAL_VISIT_DELETE, ADDITIONAL_TEST_DELETE, TREATMENT_DELETE, VISIT_DELETE, TASK_VIEW, SAMPLE_VIEW, PRESCRIPTION_DELETE, ADDITIONAL_TEST_VIEW, TASK_DELETE, PERSON_DELETE, DOCUMENT_DELETE, PERSON_VIEW, CASE_VIEW, CLINICAL_COURSE_VIEW, IMMUNIZATION_DELETE, IMMUNIZATION_VIEW</t>
+    <t>ADDITIONAL_TEST_VIEW, DOCUMENT_VIEW, THERAPY_VIEW, TASK_VIEW, SAMPLE_DELETE, PERSON_DELETE, ADDITIONAL_TEST_DELETE, CASE_VIEW, TREATMENT_DELETE, PRESCRIPTION_DELETE, TASK_DELETE, CLINICAL_VISIT_DELETE, IMMUNIZATION_VIEW, PERSON_VIEW, PATHOGEN_TEST_DELETE, CLINICAL_COURSE_VIEW, DOCUMENT_DELETE, VISIT_DELETE, SAMPLE_VIEW, IMMUNIZATION_DELETE</t>
   </si>
   <si>
     <t>Import cases into SORMAS</t>
@@ -817,7 +817,7 @@
     <t>Able to edit case investigation status</t>
   </si>
   <si>
-    <t>PERSON_EDIT, PERSON_VIEW, CASE_VIEW, CASE_EDIT</t>
+    <t>CASE_EDIT, PERSON_VIEW, PERSON_EDIT, CASE_VIEW</t>
   </si>
   <si>
     <t>Edit case classification and outcome</t>
@@ -880,7 +880,7 @@
     <t>Able to create new immunizations and vaccinations</t>
   </si>
   <si>
-    <t>PERSON_VIEW, IMMUNIZATION_VIEW</t>
+    <t>IMMUNIZATION_VIEW, PERSON_VIEW</t>
   </si>
   <si>
     <t>Edit existing immunizations and vaccinations</t>
@@ -889,7 +889,7 @@
     <t>Able to edit existing immunizations and vaccinations</t>
   </si>
   <si>
-    <t>PERSON_EDIT, PERSON_VIEW, IMMUNIZATION_VIEW</t>
+    <t>IMMUNIZATION_VIEW, PERSON_VIEW, PERSON_EDIT</t>
   </si>
   <si>
     <t>Archive immunizations</t>
@@ -904,7 +904,7 @@
     <t>Able to delete immunizations and vaccinations from the system</t>
   </si>
   <si>
-    <t>PERSON_DELETE, PERSON_VIEW, IMMUNIZATION_VIEW, VISIT_DELETE</t>
+    <t>IMMUNIZATION_VIEW, PERSON_VIEW, VISIT_DELETE, PERSON_DELETE</t>
   </si>
   <si>
     <t>Persons</t>
@@ -946,7 +946,7 @@
     <t>Able to delete person contact details</t>
   </si>
   <si>
-    <t>PERSON_EDIT, PERSON_VIEW</t>
+    <t>PERSON_VIEW, PERSON_EDIT</t>
   </si>
   <si>
     <t>Sample Testing</t>
@@ -976,7 +976,7 @@
     <t>Able to delete samples from the system</t>
   </si>
   <si>
-    <t>PATHOGEN_TEST_DELETE, SAMPLE_VIEW, ADDITIONAL_TEST_VIEW, ADDITIONAL_TEST_DELETE</t>
+    <t>ADDITIONAL_TEST_VIEW, PATHOGEN_TEST_DELETE, SAMPLE_VIEW, ADDITIONAL_TEST_DELETE</t>
   </si>
   <si>
     <t>Export samples from SORMAS</t>
@@ -991,7 +991,7 @@
     <t>Able to transfer samples to another lab</t>
   </si>
   <si>
-    <t>SAMPLE_VIEW, SAMPLE_EDIT</t>
+    <t>SAMPLE_EDIT, SAMPLE_VIEW</t>
   </si>
   <si>
     <t>Edit samples reported by other users</t>
@@ -1036,7 +1036,7 @@
     <t>Able to create new additional tests</t>
   </si>
   <si>
-    <t>SAMPLE_VIEW, ADDITIONAL_TEST_VIEW</t>
+    <t>ADDITIONAL_TEST_VIEW, SAMPLE_VIEW</t>
   </si>
   <si>
     <t>Edit existing additional tests</t>
@@ -1066,7 +1066,7 @@
     <t>Able to create new contacts</t>
   </si>
   <si>
-    <t>PERSON_VIEW, CASE_VIEW, CONTACT_VIEW</t>
+    <t>PERSON_VIEW, CONTACT_VIEW, CASE_VIEW</t>
   </si>
   <si>
     <t>Edit existing contacts</t>
@@ -1075,7 +1075,7 @@
     <t>Able to edit existing contacts</t>
   </si>
   <si>
-    <t>PERSON_EDIT, PERSON_VIEW, CASE_VIEW, CONTACT_VIEW</t>
+    <t>PERSON_VIEW, PERSON_EDIT, CONTACT_VIEW, CASE_VIEW</t>
   </si>
   <si>
     <t>Archive contacts</t>
@@ -1090,7 +1090,7 @@
     <t>Able to delete contacts from the system</t>
   </si>
   <si>
-    <t>SAMPLE_DELETE, PATHOGEN_TEST_DELETE, DOCUMENT_VIEW, ADDITIONAL_TEST_DELETE, VISIT_DELETE, TASK_VIEW, SAMPLE_VIEW, ADDITIONAL_TEST_VIEW, TASK_DELETE, PERSON_DELETE, DOCUMENT_DELETE, PERSON_VIEW, CASE_VIEW, CONTACT_VIEW</t>
+    <t>ADDITIONAL_TEST_VIEW, DOCUMENT_VIEW, TASK_VIEW, SAMPLE_DELETE, PERSON_DELETE, ADDITIONAL_TEST_DELETE, CASE_VIEW, TASK_DELETE, PERSON_VIEW, PATHOGEN_TEST_DELETE, DOCUMENT_DELETE, VISIT_DELETE, SAMPLE_VIEW, CONTACT_VIEW</t>
   </si>
   <si>
     <t>Import contacts</t>
@@ -1111,7 +1111,7 @@
     <t>Able to create resulting cases from contacts</t>
   </si>
   <si>
-    <t>PERSON_EDIT, CASE_CREATE, PERSON_VIEW, CASE_VIEW, CONTACT_EDIT, CONTACT_VIEW</t>
+    <t>CASE_CREATE, PERSON_VIEW, PERSON_EDIT, CONTACT_EDIT, CASE_VIEW, CONTACT_VIEW</t>
   </si>
   <si>
     <t>Reassign the source case of contacts</t>
@@ -1120,7 +1120,7 @@
     <t>Able to reassign the source case of contacts</t>
   </si>
   <si>
-    <t>PERSON_EDIT, PERSON_VIEW, CASE_VIEW, CONTACT_EDIT, CONTACT_VIEW</t>
+    <t>PERSON_VIEW, PERSON_EDIT, CONTACT_EDIT, CONTACT_VIEW, CASE_VIEW</t>
   </si>
   <si>
     <t>Merge contacts</t>
@@ -1216,7 +1216,7 @@
     <t>Able to delete actions from the system</t>
   </si>
   <si>
-    <t>DOCUMENT_VIEW, DOCUMENT_DELETE, EVENT_VIEW</t>
+    <t>DOCUMENT_VIEW, EVENT_VIEW, DOCUMENT_DELETE</t>
   </si>
   <si>
     <t>Edit existing actions</t>
@@ -1255,7 +1255,7 @@
     <t>Able to delete events from the system</t>
   </si>
   <si>
-    <t>ACTION_DELETE, DOCUMENT_VIEW, SAMPLE_DELETE, PATHOGEN_TEST_DELETE, EVENT_VIEW, ADDITIONAL_TEST_DELETE, EVENTPARTICIPANT_DELETE, TASK_VIEW, VISIT_DELETE, EVENTPARTICIPANT_VIEW, SAMPLE_VIEW, ADDITIONAL_TEST_VIEW, TASK_DELETE, PERSON_DELETE, DOCUMENT_DELETE, PERSON_VIEW</t>
+    <t>ADDITIONAL_TEST_VIEW, DOCUMENT_VIEW, EVENTPARTICIPANT_VIEW, EVENT_VIEW, TASK_VIEW, EVENTPARTICIPANT_DELETE, ACTION_DELETE, SAMPLE_DELETE, PERSON_DELETE, ADDITIONAL_TEST_DELETE, TASK_DELETE, PERSON_VIEW, PATHOGEN_TEST_DELETE, DOCUMENT_DELETE, SAMPLE_VIEW, VISIT_DELETE</t>
   </si>
   <si>
     <t>Import events</t>
@@ -1276,7 +1276,7 @@
     <t>Able to perform bulk operations in the event directory</t>
   </si>
   <si>
-    <t>EVENT_EDIT, EVENT_VIEW</t>
+    <t>EVENT_VIEW, EVENT_EDIT</t>
   </si>
   <si>
     <t>Can be responsible for an event</t>
@@ -1288,7 +1288,7 @@
     <t>Able to view existing event participants</t>
   </si>
   <si>
-    <t>EVENT_VIEW, PERSON_VIEW</t>
+    <t>PERSON_VIEW, EVENT_VIEW</t>
   </si>
   <si>
     <t>Create new event participants</t>
@@ -1297,7 +1297,7 @@
     <t>Able to create new event participants</t>
   </si>
   <si>
-    <t>EVENTPARTICIPANT_VIEW, EVENT_VIEW, PERSON_VIEW</t>
+    <t>PERSON_VIEW, EVENTPARTICIPANT_VIEW, EVENT_VIEW</t>
   </si>
   <si>
     <t>Edit existing event participants</t>
@@ -1306,7 +1306,7 @@
     <t>Able to edit existing event participants</t>
   </si>
   <si>
-    <t>EVENTPARTICIPANT_VIEW, PERSON_EDIT, EVENT_VIEW, PERSON_VIEW</t>
+    <t>PERSON_VIEW, EVENTPARTICIPANT_VIEW, EVENT_VIEW, PERSON_EDIT</t>
   </si>
   <si>
     <t>Event participant archive</t>
@@ -1321,7 +1321,7 @@
     <t>Able to delete event participants from the system</t>
   </si>
   <si>
-    <t>SAMPLE_DELETE, PATHOGEN_TEST_DELETE, EVENTPARTICIPANT_VIEW, SAMPLE_VIEW, ADDITIONAL_TEST_VIEW, PERSON_DELETE, EVENT_VIEW, PERSON_VIEW, ADDITIONAL_TEST_DELETE, VISIT_DELETE</t>
+    <t>PERSON_VIEW, ADDITIONAL_TEST_VIEW, PATHOGEN_TEST_DELETE, EVENTPARTICIPANT_VIEW, EVENT_VIEW, SAMPLE_VIEW, VISIT_DELETE, SAMPLE_DELETE, PERSON_DELETE, ADDITIONAL_TEST_DELETE</t>
   </si>
   <si>
     <t>Import event participants</t>
@@ -1336,7 +1336,7 @@
     <t>Able to perform bulk operations in the event participants directory</t>
   </si>
   <si>
-    <t>EVENTPARTICIPANT_VIEW, PERSON_EDIT, EVENT_VIEW, EVENTPARTICIPANT_EDIT, PERSON_VIEW</t>
+    <t>PERSON_VIEW, EVENTPARTICIPANT_VIEW, EVENT_VIEW, PERSON_EDIT, EVENTPARTICIPANT_EDIT</t>
   </si>
   <si>
     <t>Create new event groups</t>
@@ -1480,7 +1480,7 @@
     <t>Able to view contact transmission chains on the dashboard</t>
   </si>
   <si>
-    <t>DASHBOARD_CONTACT_VIEW, PERSON_VIEW, CASE_VIEW, CONTACT_VIEW</t>
+    <t>PERSON_VIEW, DASHBOARD_CONTACT_VIEW, CONTACT_VIEW, CASE_VIEW</t>
   </si>
   <si>
     <t>Access campaigns dashboard</t>
@@ -1510,7 +1510,7 @@
     <t>Able to create new prescriptions</t>
   </si>
   <si>
-    <t>THERAPY_VIEW, PERSON_VIEW, CASE_VIEW</t>
+    <t>PERSON_VIEW, THERAPY_VIEW, CASE_VIEW</t>
   </si>
   <si>
     <t>Edit existing prescriptions</t>
@@ -1555,7 +1555,7 @@
     <t>Able to edit the clinical course of cases</t>
   </si>
   <si>
-    <t>THERAPY_VIEW, PERSON_VIEW, CLINICAL_COURSE_VIEW, CASE_VIEW</t>
+    <t>PERSON_VIEW, CLINICAL_COURSE_VIEW, THERAPY_VIEW, CASE_VIEW</t>
   </si>
   <si>
     <t>Create new clinical visits</t>
@@ -1591,7 +1591,7 @@
     <t>Able to edit existing port health info</t>
   </si>
   <si>
-    <t>PORT_HEALTH_INFO_VIEW, PERSON_VIEW, CASE_VIEW</t>
+    <t>PERSON_VIEW, PORT_HEALTH_INFO_VIEW, CASE_VIEW</t>
   </si>
   <si>
     <t>Aggregated Reporting</t>
@@ -1729,7 +1729,7 @@
     <t>Able to view existing travel entries</t>
   </si>
   <si>
-    <t>TRAVEL_ENTRY_MANAGEMENT_ACCESS, PERSON_VIEW</t>
+    <t>PERSON_VIEW, TRAVEL_ENTRY_MANAGEMENT_ACCESS</t>
   </si>
   <si>
     <t>Create new travel entries</t>
@@ -1738,7 +1738,7 @@
     <t>Able to create new travel entries</t>
   </si>
   <si>
-    <t>TRAVEL_ENTRY_MANAGEMENT_ACCESS, PERSON_VIEW, TRAVEL_ENTRY_VIEW</t>
+    <t>PERSON_VIEW, TRAVEL_ENTRY_MANAGEMENT_ACCESS, TRAVEL_ENTRY_VIEW</t>
   </si>
   <si>
     <t>Edit existing travel entries</t>
@@ -1747,7 +1747,7 @@
     <t>Able to edit existing travel entries</t>
   </si>
   <si>
-    <t>TRAVEL_ENTRY_MANAGEMENT_ACCESS, PERSON_EDIT, PERSON_VIEW, TRAVEL_ENTRY_VIEW</t>
+    <t>PERSON_VIEW, TRAVEL_ENTRY_MANAGEMENT_ACCESS, TRAVEL_ENTRY_VIEW, PERSON_EDIT</t>
   </si>
   <si>
     <t>Archive travel entries</t>
@@ -1762,7 +1762,7 @@
     <t>Able to delete travel entries from the system</t>
   </si>
   <si>
-    <t>DOCUMENT_VIEW, TRAVEL_ENTRY_MANAGEMENT_ACCESS, TASK_DELETE, PERSON_DELETE, DOCUMENT_DELETE, PERSON_VIEW, TRAVEL_ENTRY_VIEW, TASK_VIEW, VISIT_DELETE</t>
+    <t>TASK_DELETE, PERSON_VIEW, DOCUMENT_VIEW, TRAVEL_ENTRY_MANAGEMENT_ACCESS, DOCUMENT_DELETE, TASK_VIEW, TRAVEL_ENTRY_VIEW, VISIT_DELETE, PERSON_DELETE</t>
   </si>
   <si>
     <t>Documents</t>
@@ -1888,7 +1888,7 @@
     <t>Able to work with messages</t>
   </si>
   <si>
-    <t>PATHOGEN_TEST_DELETE, EXTERNAL_MESSAGE_VIEW, PATHOGEN_TEST_CREATE, EVENTPARTICIPANT_CREATE, SAMPLE_EDIT, VISIT_DELETE, EVENTPARTICIPANT_VIEW, SAMPLE_VIEW, PERSON_VIEW, CONTACT_EDIT, IMMUNIZATION_EDIT, IMMUNIZATION_VIEW, CONTACT_VIEW, IMMUNIZATION_CREATE, EVENT_CREATE, EVENT_VIEW, EVENTPARTICIPANT_EDIT, CASE_CREATE, CONTACT_CREATE, SAMPLE_CREATE, CASE_EDIT, PERSON_DELETE, PERSON_EDIT, EVENT_EDIT, PATHOGEN_TEST_EDIT, CASE_VIEW, IMMUNIZATION_DELETE</t>
+    <t>CASE_EDIT, EVENTPARTICIPANT_CREATE, EVENTPARTICIPANT_VIEW, EVENT_CREATE, EVENTPARTICIPANT_EDIT, PERSON_DELETE, EXTERNAL_MESSAGE_VIEW, PATHOGEN_TEST_CREATE, IMMUNIZATION_VIEW, IMMUNIZATION_EDIT, PERSON_VIEW, SAMPLE_EDIT, VISIT_DELETE, EVENT_EDIT, SAMPLE_CREATE, CONTACT_VIEW, CASE_CREATE, EVENT_VIEW, CONTACT_EDIT, PATHOGEN_TEST_EDIT, CASE_VIEW, PATHOGEN_TEST_DELETE, CONTACT_CREATE, PERSON_EDIT, SAMPLE_VIEW, IMMUNIZATION_CREATE, IMMUNIZATION_DELETE</t>
   </si>
   <si>
     <t>Delete messages from the system</t>

</xml_diff>

<commit_message>
#10074 fixed TaskService unit tests (where working before, because user service logic was not properly working)
</commit_message>
<xml_diff>
--- a/sormas-api/src/main/resources/doc/SORMAS_User_Roles.xlsx
+++ b/sormas-api/src/main/resources/doc/SORMAS_User_Roles.xlsx
@@ -758,7 +758,7 @@
     <t>Able to create new cases</t>
   </si>
   <si>
-    <t>PERSON_VIEW, CASE_VIEW</t>
+    <t>CASE_VIEW, PERSON_VIEW</t>
   </si>
   <si>
     <t>Edit existing cases</t>
@@ -767,7 +767,7 @@
     <t>Able to edit existing cases</t>
   </si>
   <si>
-    <t>PERSON_VIEW, PERSON_EDIT, CASE_VIEW</t>
+    <t>CASE_VIEW, PERSON_VIEW, PERSON_EDIT</t>
   </si>
   <si>
     <t>Archive cases</t>
@@ -782,7 +782,7 @@
     <t>Able to delete cases from the system</t>
   </si>
   <si>
-    <t>CLINICAL_VISIT_DELETE, IMMUNIZATION_VIEW, PERSON_VIEW, TASK_DELETE, PERSON_DELETE, TREATMENT_DELETE, TASK_VIEW, PATHOGEN_TEST_DELETE, IMMUNIZATION_DELETE, SAMPLE_VIEW, ADDITIONAL_TEST_VIEW, SAMPLE_DELETE, THERAPY_VIEW, VISIT_DELETE, PRESCRIPTION_DELETE, ADDITIONAL_TEST_DELETE, CASE_VIEW, CLINICAL_COURSE_VIEW, DOCUMENT_DELETE, DOCUMENT_VIEW</t>
+    <t>CLINICAL_VISIT_DELETE, CASE_VIEW, SAMPLE_VIEW, THERAPY_VIEW, TASK_VIEW, DOCUMENT_DELETE, PRESCRIPTION_DELETE, IMMUNIZATION_DELETE, TASK_DELETE, PERSON_VIEW, SAMPLE_DELETE, PERSON_DELETE, IMMUNIZATION_VIEW, VISIT_DELETE, TREATMENT_DELETE, DOCUMENT_VIEW, PATHOGEN_TEST_DELETE, ADDITIONAL_TEST_VIEW, CLINICAL_COURSE_VIEW, ADDITIONAL_TEST_DELETE</t>
   </si>
   <si>
     <t>Import cases into SORMAS</t>
@@ -803,7 +803,7 @@
     <t>Able to edit case investigation status</t>
   </si>
   <si>
-    <t>PERSON_VIEW, CASE_EDIT, PERSON_EDIT, CASE_VIEW</t>
+    <t>CASE_EDIT, CASE_VIEW, PERSON_VIEW, PERSON_EDIT</t>
   </si>
   <si>
     <t>Edit case classification and outcome</t>
@@ -866,7 +866,7 @@
     <t>Able to create new immunizations and vaccinations</t>
   </si>
   <si>
-    <t>IMMUNIZATION_VIEW, PERSON_VIEW</t>
+    <t>PERSON_VIEW, IMMUNIZATION_VIEW</t>
   </si>
   <si>
     <t>Edit existing immunizations and vaccinations</t>
@@ -875,7 +875,7 @@
     <t>Able to edit existing immunizations and vaccinations</t>
   </si>
   <si>
-    <t>IMMUNIZATION_VIEW, PERSON_VIEW, PERSON_EDIT</t>
+    <t>PERSON_VIEW, IMMUNIZATION_VIEW, PERSON_EDIT</t>
   </si>
   <si>
     <t>Archive immunizations</t>
@@ -890,7 +890,7 @@
     <t>Able to delete immunizations and vaccinations from the system</t>
   </si>
   <si>
-    <t>IMMUNIZATION_VIEW, PERSON_VIEW, PERSON_DELETE, VISIT_DELETE</t>
+    <t>PERSON_VIEW, PERSON_DELETE, IMMUNIZATION_VIEW, VISIT_DELETE</t>
   </si>
   <si>
     <t>Persons</t>
@@ -965,7 +965,7 @@
     <t>Able to delete samples from the system</t>
   </si>
   <si>
-    <t>ADDITIONAL_TEST_DELETE, PATHOGEN_TEST_DELETE, SAMPLE_VIEW, ADDITIONAL_TEST_VIEW</t>
+    <t>SAMPLE_VIEW, PATHOGEN_TEST_DELETE, ADDITIONAL_TEST_VIEW, ADDITIONAL_TEST_DELETE</t>
   </si>
   <si>
     <t>Export samples from SORMAS</t>
@@ -980,7 +980,7 @@
     <t>Able to transfer samples to another lab</t>
   </si>
   <si>
-    <t>SAMPLE_EDIT, SAMPLE_VIEW</t>
+    <t>SAMPLE_VIEW, SAMPLE_EDIT</t>
   </si>
   <si>
     <t>Edit samples reported by other users</t>
@@ -1055,7 +1055,7 @@
     <t>Able to create new contacts</t>
   </si>
   <si>
-    <t>PERSON_VIEW, CONTACT_VIEW, CASE_VIEW</t>
+    <t>CASE_VIEW, PERSON_VIEW, CONTACT_VIEW</t>
   </si>
   <si>
     <t>Edit existing contacts</t>
@@ -1064,7 +1064,7 @@
     <t>Able to edit existing contacts</t>
   </si>
   <si>
-    <t>PERSON_VIEW, PERSON_EDIT, CONTACT_VIEW, CASE_VIEW</t>
+    <t>CASE_VIEW, PERSON_VIEW, CONTACT_VIEW, PERSON_EDIT</t>
   </si>
   <si>
     <t>Archive contacts</t>
@@ -1079,7 +1079,7 @@
     <t>Able to delete contacts from the system</t>
   </si>
   <si>
-    <t>PERSON_VIEW, TASK_DELETE, PERSON_DELETE, CONTACT_VIEW, TASK_VIEW, PATHOGEN_TEST_DELETE, SAMPLE_VIEW, ADDITIONAL_TEST_VIEW, SAMPLE_DELETE, VISIT_DELETE, ADDITIONAL_TEST_DELETE, CASE_VIEW, DOCUMENT_DELETE, DOCUMENT_VIEW</t>
+    <t>CASE_VIEW, SAMPLE_VIEW, TASK_VIEW, DOCUMENT_DELETE, CONTACT_VIEW, TASK_DELETE, PERSON_VIEW, SAMPLE_DELETE, PERSON_DELETE, VISIT_DELETE, DOCUMENT_VIEW, PATHOGEN_TEST_DELETE, ADDITIONAL_TEST_VIEW, ADDITIONAL_TEST_DELETE</t>
   </si>
   <si>
     <t>Import contacts</t>
@@ -1100,7 +1100,7 @@
     <t>Able to create resulting cases from contacts</t>
   </si>
   <si>
-    <t>PERSON_VIEW, PERSON_EDIT, CONTACT_VIEW, CASE_CREATE, CONTACT_EDIT, CASE_VIEW</t>
+    <t>CONTACT_EDIT, CASE_VIEW, PERSON_VIEW, CASE_CREATE, CONTACT_VIEW, PERSON_EDIT</t>
   </si>
   <si>
     <t>Reassign the source case of contacts</t>
@@ -1109,7 +1109,7 @@
     <t>Able to reassign the source case of contacts</t>
   </si>
   <si>
-    <t>PERSON_VIEW, PERSON_EDIT, CONTACT_VIEW, CONTACT_EDIT, CASE_VIEW</t>
+    <t>CONTACT_EDIT, CASE_VIEW, PERSON_VIEW, CONTACT_VIEW, PERSON_EDIT</t>
   </si>
   <si>
     <t>Merge contacts</t>
@@ -1250,7 +1250,7 @@
     <t>Able to delete events from the system</t>
   </si>
   <si>
-    <t>PERSON_VIEW, TASK_DELETE, PERSON_DELETE, TASK_VIEW, EVENTPARTICIPANT_VIEW, PATHOGEN_TEST_DELETE, SAMPLE_VIEW, ADDITIONAL_TEST_VIEW, ACTION_DELETE, EVENT_VIEW, SAMPLE_DELETE, VISIT_DELETE, ADDITIONAL_TEST_DELETE, EVENTPARTICIPANT_DELETE, DOCUMENT_DELETE, DOCUMENT_VIEW</t>
+    <t>SAMPLE_VIEW, TASK_VIEW, DOCUMENT_DELETE, EVENTPARTICIPANT_DELETE, EVENTPARTICIPANT_VIEW, TASK_DELETE, PERSON_VIEW, SAMPLE_DELETE, PERSON_DELETE, EVENT_VIEW, ACTION_DELETE, DOCUMENT_VIEW, VISIT_DELETE, PATHOGEN_TEST_DELETE, ADDITIONAL_TEST_VIEW, ADDITIONAL_TEST_DELETE</t>
   </si>
   <si>
     <t>Import events</t>
@@ -1292,7 +1292,7 @@
     <t>Able to create new event participants</t>
   </si>
   <si>
-    <t>PERSON_VIEW, EVENTPARTICIPANT_VIEW, EVENT_VIEW</t>
+    <t>PERSON_VIEW, EVENT_VIEW, EVENTPARTICIPANT_VIEW</t>
   </si>
   <si>
     <t>Edit existing event participants</t>
@@ -1301,7 +1301,7 @@
     <t>Able to edit existing event participants</t>
   </si>
   <si>
-    <t>PERSON_VIEW, PERSON_EDIT, EVENTPARTICIPANT_VIEW, EVENT_VIEW</t>
+    <t>PERSON_VIEW, EVENT_VIEW, EVENTPARTICIPANT_VIEW, PERSON_EDIT</t>
   </si>
   <si>
     <t>Event participant archive</t>
@@ -1316,7 +1316,7 @@
     <t>Able to delete event participants from the system</t>
   </si>
   <si>
-    <t>SAMPLE_DELETE, PERSON_VIEW, PERSON_DELETE, VISIT_DELETE, ADDITIONAL_TEST_DELETE, EVENTPARTICIPANT_VIEW, PATHOGEN_TEST_DELETE, SAMPLE_VIEW, ADDITIONAL_TEST_VIEW, EVENT_VIEW</t>
+    <t>PERSON_VIEW, SAMPLE_VIEW, SAMPLE_DELETE, PERSON_DELETE, EVENT_VIEW, VISIT_DELETE, PATHOGEN_TEST_DELETE, ADDITIONAL_TEST_VIEW, EVENTPARTICIPANT_VIEW, ADDITIONAL_TEST_DELETE</t>
   </si>
   <si>
     <t>Import event participants</t>
@@ -1331,7 +1331,7 @@
     <t>Able to perform bulk operations in the event participants directory</t>
   </si>
   <si>
-    <t>PERSON_VIEW, PERSON_EDIT, EVENTPARTICIPANT_VIEW, EVENTPARTICIPANT_EDIT, EVENT_VIEW</t>
+    <t>PERSON_VIEW, EVENTPARTICIPANT_EDIT, EVENT_VIEW, EVENTPARTICIPANT_VIEW, PERSON_EDIT</t>
   </si>
   <si>
     <t>Create new event groups</t>
@@ -1475,7 +1475,7 @@
     <t>Able to view contact transmission chains on the dashboard</t>
   </si>
   <si>
-    <t>PERSON_VIEW, DASHBOARD_CONTACT_VIEW, CONTACT_VIEW, CASE_VIEW</t>
+    <t>DASHBOARD_CONTACT_VIEW, CASE_VIEW, PERSON_VIEW, CONTACT_VIEW</t>
   </si>
   <si>
     <t>Access campaigns dashboard</t>
@@ -1505,7 +1505,7 @@
     <t>Able to create new prescriptions</t>
   </si>
   <si>
-    <t>THERAPY_VIEW, PERSON_VIEW, CASE_VIEW</t>
+    <t>CASE_VIEW, PERSON_VIEW, THERAPY_VIEW</t>
   </si>
   <si>
     <t>Edit existing prescriptions</t>
@@ -1550,7 +1550,7 @@
     <t>Able to edit the clinical course of cases</t>
   </si>
   <si>
-    <t>THERAPY_VIEW, PERSON_VIEW, CLINICAL_COURSE_VIEW, CASE_VIEW</t>
+    <t>CASE_VIEW, PERSON_VIEW, THERAPY_VIEW, CLINICAL_COURSE_VIEW</t>
   </si>
   <si>
     <t>Create new clinical visits</t>
@@ -1586,7 +1586,7 @@
     <t>Able to edit existing port health info</t>
   </si>
   <si>
-    <t>PERSON_VIEW, PORT_HEALTH_INFO_VIEW, CASE_VIEW</t>
+    <t>CASE_VIEW, PERSON_VIEW, PORT_HEALTH_INFO_VIEW</t>
   </si>
   <si>
     <t>Aggregated Reporting</t>
@@ -1676,7 +1676,7 @@
     <t>Able to delete campaigns from the system</t>
   </si>
   <si>
-    <t>CAMPAIGN_FORM_DATA_VIEW, CAMPAIGN_VIEW, CAMPAIGN_FORM_DATA_DELETE</t>
+    <t>CAMPAIGN_VIEW, CAMPAIGN_FORM_DATA_VIEW, CAMPAIGN_FORM_DATA_DELETE</t>
   </si>
   <si>
     <t>View existing campaign form data</t>
@@ -1724,7 +1724,7 @@
     <t>Able to view existing travel entries</t>
   </si>
   <si>
-    <t>TRAVEL_ENTRY_MANAGEMENT_ACCESS, PERSON_VIEW</t>
+    <t>PERSON_VIEW, TRAVEL_ENTRY_MANAGEMENT_ACCESS</t>
   </si>
   <si>
     <t>Create new travel entries</t>
@@ -1733,7 +1733,7 @@
     <t>Able to create new travel entries</t>
   </si>
   <si>
-    <t>TRAVEL_ENTRY_MANAGEMENT_ACCESS, PERSON_VIEW, TRAVEL_ENTRY_VIEW</t>
+    <t>PERSON_VIEW, TRAVEL_ENTRY_MANAGEMENT_ACCESS, TRAVEL_ENTRY_VIEW</t>
   </si>
   <si>
     <t>Edit existing travel entries</t>
@@ -1742,7 +1742,7 @@
     <t>Able to edit existing travel entries</t>
   </si>
   <si>
-    <t>TRAVEL_ENTRY_MANAGEMENT_ACCESS, PERSON_VIEW, PERSON_EDIT, TRAVEL_ENTRY_VIEW</t>
+    <t>PERSON_VIEW, TRAVEL_ENTRY_MANAGEMENT_ACCESS, TRAVEL_ENTRY_VIEW, PERSON_EDIT</t>
   </si>
   <si>
     <t>Archive travel entries</t>
@@ -1757,7 +1757,7 @@
     <t>Able to delete travel entries from the system</t>
   </si>
   <si>
-    <t>TRAVEL_ENTRY_MANAGEMENT_ACCESS, PERSON_VIEW, TASK_DELETE, PERSON_DELETE, VISIT_DELETE, TRAVEL_ENTRY_VIEW, TASK_VIEW, DOCUMENT_DELETE, DOCUMENT_VIEW</t>
+    <t>PERSON_VIEW, PERSON_DELETE, TASK_VIEW, DOCUMENT_DELETE, VISIT_DELETE, DOCUMENT_VIEW, TRAVEL_ENTRY_MANAGEMENT_ACCESS, TRAVEL_ENTRY_VIEW, TASK_DELETE</t>
   </si>
   <si>
     <t>Documents</t>
@@ -1883,7 +1883,7 @@
     <t>Able to work with messages</t>
   </si>
   <si>
-    <t>PERSON_DELETE, EVENT_CREATE, CASE_EDIT, PATHOGEN_TEST_EDIT, IMMUNIZATION_DELETE, SAMPLE_VIEW, EVENT_VIEW, IMMUNIZATION_EDIT, CONTACT_CREATE, EXTERNAL_MESSAGE_VIEW, SAMPLE_EDIT, CASE_CREATE, EVENTPARTICIPANT_EDIT, EVENT_EDIT, IMMUNIZATION_VIEW, PERSON_VIEW, PERSON_EDIT, CONTACT_VIEW, PATHOGEN_TEST_DELETE, EVENTPARTICIPANT_VIEW, PATHOGEN_TEST_CREATE, CONTACT_EDIT, VISIT_DELETE, EVENTPARTICIPANT_CREATE, SAMPLE_CREATE, IMMUNIZATION_CREATE, CASE_VIEW</t>
+    <t>SAMPLE_VIEW, EVENTPARTICIPANT_EDIT, CONTACT_CREATE, PATHOGEN_TEST_EDIT, SAMPLE_EDIT, CONTACT_VIEW, IMMUNIZATION_EDIT, CONTACT_EDIT, EXTERNAL_MESSAGE_VIEW, PERSON_VIEW, SAMPLE_CREATE, EVENT_VIEW, PATHOGEN_TEST_DELETE, EVENT_EDIT, CASE_VIEW, EVENT_CREATE, CASE_CREATE, PATHOGEN_TEST_CREATE, IMMUNIZATION_DELETE, EVENTPARTICIPANT_VIEW, CASE_EDIT, PERSON_DELETE, EVENTPARTICIPANT_CREATE, IMMUNIZATION_CREATE, IMMUNIZATION_VIEW, VISIT_DELETE, PERSON_EDIT</t>
   </si>
   <si>
     <t>Delete messages from the system</t>
@@ -2051,7 +2051,7 @@
     <t>SORMAS Version</t>
   </si>
   <si>
-    <t>1.78.0-SNAPSHOT</t>
+    <t>1.0.0</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
#11715 - Users limited by a disease should not be able to delete and edit entities of other diseases
</commit_message>
<xml_diff>
--- a/sormas-api/src/main/resources/doc/SORMAS_User_Roles.xlsx
+++ b/sormas-api/src/main/resources/doc/SORMAS_User_Roles.xlsx
@@ -791,7 +791,7 @@
     <t>Able to delete cases from the system</t>
   </si>
   <si>
-    <t>IMMUNIZATION_VIEW, PRESCRIPTION_DELETE, PERSON_VIEW, ADDITIONAL_TEST_VIEW, SAMPLE_DELETE, CLINICAL_VISIT_DELETE, SAMPLE_VIEW, TREATMENT_DELETE, IMMUNIZATION_DELETE, TASK_VIEW, VISIT_DELETE, CLINICAL_COURSE_VIEW, THERAPY_VIEW, DOCUMENT_VIEW, TASK_DELETE, ADDITIONAL_TEST_DELETE, PERSON_DELETE, PATHOGEN_TEST_DELETE, DOCUMENT_DELETE, CASE_VIEW</t>
+    <t>CLINICAL_VISIT_DELETE, CLINICAL_COURSE_VIEW, TREATMENT_DELETE, ADDITIONAL_TEST_DELETE, IMMUNIZATION_DELETE, TASK_VIEW, CASE_VIEW, DOCUMENT_DELETE, PERSON_DELETE, PRESCRIPTION_DELETE, TASK_DELETE, PERSON_VIEW, DOCUMENT_VIEW, PATHOGEN_TEST_DELETE, VISIT_DELETE, SAMPLE_DELETE, ADDITIONAL_TEST_VIEW, SAMPLE_VIEW, THERAPY_VIEW, IMMUNIZATION_VIEW</t>
   </si>
   <si>
     <t>Import cases into SORMAS</t>
@@ -812,7 +812,7 @@
     <t>Able to edit case investigation status</t>
   </si>
   <si>
-    <t>PERSON_VIEW, PERSON_EDIT, CASE_VIEW, CASE_EDIT</t>
+    <t>PERSON_VIEW, CASE_EDIT, PERSON_EDIT, CASE_VIEW</t>
   </si>
   <si>
     <t>Edit case classification and outcome</t>
@@ -875,7 +875,7 @@
     <t>Able to create new immunizations and vaccinations</t>
   </si>
   <si>
-    <t>IMMUNIZATION_VIEW, PERSON_VIEW</t>
+    <t>PERSON_VIEW, IMMUNIZATION_VIEW</t>
   </si>
   <si>
     <t>Edit existing immunizations and vaccinations</t>
@@ -884,7 +884,7 @@
     <t>Able to edit existing immunizations and vaccinations</t>
   </si>
   <si>
-    <t>IMMUNIZATION_VIEW, PERSON_VIEW, PERSON_EDIT</t>
+    <t>PERSON_VIEW, PERSON_EDIT, IMMUNIZATION_VIEW</t>
   </si>
   <si>
     <t>Archive immunizations</t>
@@ -899,7 +899,7 @@
     <t>Able to delete immunizations and vaccinations from the system</t>
   </si>
   <si>
-    <t>IMMUNIZATION_VIEW, VISIT_DELETE, PERSON_VIEW, PERSON_DELETE</t>
+    <t>PERSON_VIEW, VISIT_DELETE, PERSON_DELETE, IMMUNIZATION_VIEW</t>
   </si>
   <si>
     <t>Persons</t>
@@ -923,7 +923,7 @@
     <t>Able to delete persons from the system</t>
   </si>
   <si>
-    <t>VISIT_DELETE, PERSON_VIEW</t>
+    <t>PERSON_VIEW, VISIT_DELETE</t>
   </si>
   <si>
     <t>Export persons</t>
@@ -974,7 +974,7 @@
     <t>Able to delete samples from the system</t>
   </si>
   <si>
-    <t>ADDITIONAL_TEST_DELETE, ADDITIONAL_TEST_VIEW, PATHOGEN_TEST_DELETE, SAMPLE_VIEW</t>
+    <t>PATHOGEN_TEST_DELETE, ADDITIONAL_TEST_VIEW, SAMPLE_VIEW, ADDITIONAL_TEST_DELETE</t>
   </si>
   <si>
     <t>Export samples from SORMAS</t>
@@ -989,7 +989,7 @@
     <t>Able to transfer samples to another lab</t>
   </si>
   <si>
-    <t>SAMPLE_EDIT, SAMPLE_VIEW</t>
+    <t>SAMPLE_VIEW, SAMPLE_EDIT</t>
   </si>
   <si>
     <t>Edit samples reported by other users</t>
@@ -1064,7 +1064,7 @@
     <t>Able to create new contacts</t>
   </si>
   <si>
-    <t>PERSON_VIEW, CASE_VIEW, CONTACT_VIEW</t>
+    <t>PERSON_VIEW, CONTACT_VIEW, CASE_VIEW</t>
   </si>
   <si>
     <t>Edit existing contacts</t>
@@ -1073,7 +1073,7 @@
     <t>Able to edit existing contacts</t>
   </si>
   <si>
-    <t>PERSON_VIEW, PERSON_EDIT, CASE_VIEW, CONTACT_VIEW</t>
+    <t>PERSON_VIEW, CONTACT_VIEW, PERSON_EDIT, CASE_VIEW</t>
   </si>
   <si>
     <t>Archive contacts</t>
@@ -1088,7 +1088,7 @@
     <t>Able to delete contacts from the system</t>
   </si>
   <si>
-    <t>PERSON_VIEW, ADDITIONAL_TEST_VIEW, SAMPLE_DELETE, SAMPLE_VIEW, CONTACT_VIEW, TASK_VIEW, VISIT_DELETE, DOCUMENT_VIEW, TASK_DELETE, ADDITIONAL_TEST_DELETE, PERSON_DELETE, PATHOGEN_TEST_DELETE, DOCUMENT_DELETE, CASE_VIEW</t>
+    <t>ADDITIONAL_TEST_DELETE, TASK_VIEW, CASE_VIEW, DOCUMENT_DELETE, PERSON_DELETE, TASK_DELETE, PERSON_VIEW, DOCUMENT_VIEW, CONTACT_VIEW, PATHOGEN_TEST_DELETE, VISIT_DELETE, SAMPLE_DELETE, ADDITIONAL_TEST_VIEW, SAMPLE_VIEW</t>
   </si>
   <si>
     <t>Import contacts</t>
@@ -1109,7 +1109,7 @@
     <t>Able to create resulting cases from contacts</t>
   </si>
   <si>
-    <t>CONTACT_EDIT, PERSON_VIEW, PERSON_EDIT, CASE_VIEW, CASE_CREATE, CONTACT_VIEW</t>
+    <t>PERSON_VIEW, CONTACT_EDIT, CONTACT_VIEW, PERSON_EDIT, CASE_VIEW, CASE_CREATE</t>
   </si>
   <si>
     <t>Reassign the source case of contacts</t>
@@ -1118,7 +1118,7 @@
     <t>Able to reassign the source case of contacts</t>
   </si>
   <si>
-    <t>CONTACT_EDIT, PERSON_VIEW, PERSON_EDIT, CASE_VIEW, CONTACT_VIEW</t>
+    <t>PERSON_VIEW, CONTACT_EDIT, CONTACT_VIEW, PERSON_EDIT, CASE_VIEW</t>
   </si>
   <si>
     <t>Merge contacts</t>
@@ -1196,7 +1196,7 @@
     <t>Able to assign tasks to users</t>
   </si>
   <si>
-    <t>TASK_VIEW, TASK_EDIT</t>
+    <t>TASK_EDIT, TASK_VIEW</t>
   </si>
   <si>
     <t>Archive tasks</t>
@@ -1259,7 +1259,7 @@
     <t>Able to delete events from the system</t>
   </si>
   <si>
-    <t>PERSON_VIEW, ADDITIONAL_TEST_VIEW, SAMPLE_DELETE, SAMPLE_VIEW, EVENTPARTICIPANT_DELETE, TASK_VIEW, VISIT_DELETE, ACTION_DELETE, DOCUMENT_VIEW, TASK_DELETE, ADDITIONAL_TEST_DELETE, EVENTPARTICIPANT_VIEW, PERSON_DELETE, PATHOGEN_TEST_DELETE, EVENT_VIEW, DOCUMENT_DELETE</t>
+    <t>ADDITIONAL_TEST_DELETE, ACTION_DELETE, TASK_VIEW, DOCUMENT_DELETE, PERSON_DELETE, TASK_DELETE, PERSON_VIEW, DOCUMENT_VIEW, PATHOGEN_TEST_DELETE, VISIT_DELETE, EVENT_VIEW, SAMPLE_DELETE, ADDITIONAL_TEST_VIEW, EVENTPARTICIPANT_DELETE, EVENTPARTICIPANT_VIEW, SAMPLE_VIEW</t>
   </si>
   <si>
     <t>Import events</t>
@@ -1301,7 +1301,7 @@
     <t>Able to create new event participants</t>
   </si>
   <si>
-    <t>PERSON_VIEW, EVENTPARTICIPANT_VIEW, EVENT_VIEW</t>
+    <t>PERSON_VIEW, EVENT_VIEW, EVENTPARTICIPANT_VIEW</t>
   </si>
   <si>
     <t>Edit existing event participants</t>
@@ -1310,7 +1310,7 @@
     <t>Able to edit existing event participants</t>
   </si>
   <si>
-    <t>PERSON_VIEW, PERSON_EDIT, EVENTPARTICIPANT_VIEW, EVENT_VIEW</t>
+    <t>PERSON_VIEW, PERSON_EDIT, EVENT_VIEW, EVENTPARTICIPANT_VIEW</t>
   </si>
   <si>
     <t>Event participant archive</t>
@@ -1325,7 +1325,7 @@
     <t>Able to delete event participants from the system</t>
   </si>
   <si>
-    <t>VISIT_DELETE, PERSON_VIEW, ADDITIONAL_TEST_DELETE, ADDITIONAL_TEST_VIEW, EVENTPARTICIPANT_VIEW, PERSON_DELETE, PATHOGEN_TEST_DELETE, EVENT_VIEW, SAMPLE_DELETE, SAMPLE_VIEW</t>
+    <t>PERSON_VIEW, PATHOGEN_TEST_DELETE, VISIT_DELETE, SAMPLE_DELETE, ADDITIONAL_TEST_VIEW, EVENT_VIEW, EVENTPARTICIPANT_VIEW, SAMPLE_VIEW, ADDITIONAL_TEST_DELETE, PERSON_DELETE</t>
   </si>
   <si>
     <t>Import event participants</t>
@@ -1340,7 +1340,7 @@
     <t>Able to perform bulk operations in the event participants directory</t>
   </si>
   <si>
-    <t>EVENTPARTICIPANT_EDIT, PERSON_VIEW, PERSON_EDIT, EVENTPARTICIPANT_VIEW, EVENT_VIEW</t>
+    <t>PERSON_VIEW, EVENTPARTICIPANT_EDIT, PERSON_EDIT, EVENT_VIEW, EVENTPARTICIPANT_VIEW</t>
   </si>
   <si>
     <t>Create new event groups</t>
@@ -1484,7 +1484,7 @@
     <t>Able to view contact transmission chains on the dashboard</t>
   </si>
   <si>
-    <t>DASHBOARD_CONTACT_VIEW, PERSON_VIEW, CASE_VIEW, CONTACT_VIEW</t>
+    <t>PERSON_VIEW, DASHBOARD_CONTACT_VIEW, CONTACT_VIEW, CASE_VIEW</t>
   </si>
   <si>
     <t>Access campaigns dashboard</t>
@@ -1517,7 +1517,7 @@
     <t>Able to create new prescriptions</t>
   </si>
   <si>
-    <t>THERAPY_VIEW, PERSON_VIEW, CASE_VIEW</t>
+    <t>PERSON_VIEW, THERAPY_VIEW, CASE_VIEW</t>
   </si>
   <si>
     <t>Edit existing prescriptions</t>
@@ -1562,7 +1562,7 @@
     <t>Able to edit the clinical course of cases</t>
   </si>
   <si>
-    <t>CLINICAL_COURSE_VIEW, THERAPY_VIEW, PERSON_VIEW, CASE_VIEW</t>
+    <t>PERSON_VIEW, CLINICAL_COURSE_VIEW, THERAPY_VIEW, CASE_VIEW</t>
   </si>
   <si>
     <t>Create new clinical visits</t>
@@ -1688,7 +1688,7 @@
     <t>Able to delete campaigns from the system</t>
   </si>
   <si>
-    <t>CAMPAIGN_VIEW, CAMPAIGN_FORM_DATA_VIEW, CAMPAIGN_FORM_DATA_DELETE</t>
+    <t>CAMPAIGN_VIEW, CAMPAIGN_FORM_DATA_DELETE, CAMPAIGN_FORM_DATA_VIEW</t>
   </si>
   <si>
     <t>View existing campaign form data</t>
@@ -1736,7 +1736,7 @@
     <t>Able to view existing travel entries</t>
   </si>
   <si>
-    <t>TRAVEL_ENTRY_MANAGEMENT_ACCESS, PERSON_VIEW</t>
+    <t>PERSON_VIEW, TRAVEL_ENTRY_MANAGEMENT_ACCESS</t>
   </si>
   <si>
     <t>Create new travel entries</t>
@@ -1745,7 +1745,7 @@
     <t>Able to create new travel entries</t>
   </si>
   <si>
-    <t>TRAVEL_ENTRY_VIEW, TRAVEL_ENTRY_MANAGEMENT_ACCESS, PERSON_VIEW</t>
+    <t>PERSON_VIEW, TRAVEL_ENTRY_MANAGEMENT_ACCESS, TRAVEL_ENTRY_VIEW</t>
   </si>
   <si>
     <t>Edit existing travel entries</t>
@@ -1754,7 +1754,7 @@
     <t>Able to edit existing travel entries</t>
   </si>
   <si>
-    <t>TRAVEL_ENTRY_VIEW, TRAVEL_ENTRY_MANAGEMENT_ACCESS, PERSON_VIEW, PERSON_EDIT</t>
+    <t>PERSON_VIEW, TRAVEL_ENTRY_MANAGEMENT_ACCESS, TRAVEL_ENTRY_VIEW, PERSON_EDIT</t>
   </si>
   <si>
     <t>Archive travel entries</t>
@@ -1769,7 +1769,7 @@
     <t>Able to delete travel entries from the system</t>
   </si>
   <si>
-    <t>TASK_VIEW, TRAVEL_ENTRY_VIEW, VISIT_DELETE, TRAVEL_ENTRY_MANAGEMENT_ACCESS, DOCUMENT_VIEW, PERSON_VIEW, TASK_DELETE, PERSON_DELETE, DOCUMENT_DELETE</t>
+    <t>PERSON_VIEW, DOCUMENT_VIEW, TRAVEL_ENTRY_MANAGEMENT_ACCESS, VISIT_DELETE, TRAVEL_ENTRY_VIEW, TASK_VIEW, DOCUMENT_DELETE, PERSON_DELETE, TASK_DELETE</t>
   </si>
   <si>
     <t>Documents</t>
@@ -1907,7 +1907,7 @@
     <t>Able to work with messages</t>
   </si>
   <si>
-    <t>CONTACT_EDIT, IMMUNIZATION_VIEW, PERSON_VIEW, PERSON_EDIT, SAMPLE_VIEW, CASE_CREATE, PATHOGEN_TEST_EDIT, EVENTPARTICIPANT_EDIT, SAMPLE_CREATE, PATHOGEN_TEST_DELETE, EVENT_EDIT, EVENT_VIEW, EVENTPARTICIPANT_CREATE, CASE_EDIT, PATHOGEN_TEST_CREATE, CONTACT_VIEW, IMMUNIZATION_CREATE, EXTERNAL_MESSAGE_VIEW, SAMPLE_EDIT, IMMUNIZATION_DELETE, VISIT_DELETE, EVENTPARTICIPANT_VIEW, PERSON_DELETE, CONTACT_CREATE, EVENT_CREATE, CASE_VIEW, IMMUNIZATION_EDIT</t>
+    <t>PATHOGEN_TEST_EDIT, EVENTPARTICIPANT_EDIT, CASE_VIEW, CASE_CREATE, SAMPLE_EDIT, PERSON_DELETE, PERSON_VIEW, CONTACT_EDIT, VISIT_DELETE, CASE_EDIT, SAMPLE_VIEW, EVENTPARTICIPANT_VIEW, IMMUNIZATION_VIEW, CONTACT_CREATE, EXTERNAL_MESSAGE_VIEW, PATHOGEN_TEST_CREATE, EVENT_EDIT, IMMUNIZATION_EDIT, EVENTPARTICIPANT_CREATE, SAMPLE_CREATE, PERSON_EDIT, IMMUNIZATION_DELETE, CONTACT_VIEW, PATHOGEN_TEST_DELETE, EVENT_VIEW, EVENT_CREATE, IMMUNIZATION_CREATE</t>
   </si>
   <si>
     <t>Delete messages from the system</t>
@@ -2075,7 +2075,7 @@
     <t>SORMAS Version</t>
   </si>
   <si>
-    <t>1.83.0-SNAPSHOT</t>
+    <t>1.0.0</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
#13029 - Search by NationalID is not consistently working in all locations
</commit_message>
<xml_diff>
--- a/sormas-api/src/main/resources/doc/SORMAS_User_Roles.xlsx
+++ b/sormas-api/src/main/resources/doc/SORMAS_User_Roles.xlsx
@@ -830,7 +830,7 @@
     <t>Able to create new cases</t>
   </si>
   <si>
-    <t>PERSON_VIEW, CASE_VIEW</t>
+    <t>CASE_VIEW, PERSON_VIEW</t>
   </si>
   <si>
     <t>Edit existing cases</t>
@@ -839,7 +839,7 @@
     <t>Able to edit existing cases</t>
   </si>
   <si>
-    <t>PERSON_VIEW, CASE_VIEW, PERSON_EDIT</t>
+    <t>CASE_VIEW, PERSON_VIEW, PERSON_EDIT</t>
   </si>
   <si>
     <t>Archive cases</t>
@@ -854,7 +854,7 @@
     <t>Able to delete cases from the system</t>
   </si>
   <si>
-    <t>ADDITIONAL_TEST_DELETE, PATHOGEN_TEST_DELETE, TASK_VIEW, PRESCRIPTION_DELETE, CLINICAL_VISIT_DELETE, THERAPY_VIEW, IMMUNIZATION_DELETE, DOCUMENT_VIEW, SAMPLE_DELETE, PERSON_VIEW, DOCUMENT_DELETE, IMMUNIZATION_VIEW, PERSON_DELETE, CASE_VIEW, TASK_DELETE, SAMPLE_VIEW, CLINICAL_COURSE_VIEW, ADDITIONAL_TEST_VIEW, VISIT_DELETE, TREATMENT_DELETE</t>
+    <t>SAMPLE_VIEW, ADDITIONAL_TEST_VIEW, DOCUMENT_VIEW, VISIT_DELETE, CLINICAL_COURSE_VIEW, IMMUNIZATION_VIEW, DOCUMENT_DELETE, IMMUNIZATION_DELETE, TASK_DELETE, TASK_VIEW, PERSON_VIEW, PERSON_DELETE, PATHOGEN_TEST_DELETE, PRESCRIPTION_DELETE, CLINICAL_VISIT_DELETE, CASE_VIEW, ADDITIONAL_TEST_DELETE, SAMPLE_DELETE, THERAPY_VIEW, TREATMENT_DELETE</t>
   </si>
   <si>
     <t>Import cases into SORMAS</t>
@@ -875,7 +875,7 @@
     <t>Able to edit case investigation status</t>
   </si>
   <si>
-    <t>CASE_EDIT, PERSON_VIEW, CASE_VIEW, PERSON_EDIT</t>
+    <t>CASE_VIEW, CASE_EDIT, PERSON_VIEW, PERSON_EDIT</t>
   </si>
   <si>
     <t>Edit case classification and outcome</t>
@@ -944,7 +944,7 @@
     <t>Able to create new immunizations and vaccinations</t>
   </si>
   <si>
-    <t>PERSON_VIEW, IMMUNIZATION_VIEW</t>
+    <t>IMMUNIZATION_VIEW, PERSON_VIEW</t>
   </si>
   <si>
     <t>Edit existing immunizations and vaccinations</t>
@@ -953,7 +953,7 @@
     <t>Able to edit existing immunizations and vaccinations</t>
   </si>
   <si>
-    <t>PERSON_VIEW, IMMUNIZATION_VIEW, PERSON_EDIT</t>
+    <t>IMMUNIZATION_VIEW, PERSON_VIEW, PERSON_EDIT</t>
   </si>
   <si>
     <t>Archive immunizations</t>
@@ -968,7 +968,7 @@
     <t>Able to delete immunizations and vaccinations from the system</t>
   </si>
   <si>
-    <t>PERSON_VIEW, IMMUNIZATION_VIEW, PERSON_DELETE, VISIT_DELETE</t>
+    <t>VISIT_DELETE, IMMUNIZATION_VIEW, PERSON_VIEW, PERSON_DELETE</t>
   </si>
   <si>
     <t>Persons</t>
@@ -992,7 +992,7 @@
     <t>Able to delete persons from the system</t>
   </si>
   <si>
-    <t>PERSON_VIEW, VISIT_DELETE</t>
+    <t>VISIT_DELETE, PERSON_VIEW</t>
   </si>
   <si>
     <t>Export persons</t>
@@ -1043,7 +1043,7 @@
     <t>Able to delete samples from the system</t>
   </si>
   <si>
-    <t>ADDITIONAL_TEST_DELETE, PATHOGEN_TEST_DELETE, SAMPLE_VIEW, ADDITIONAL_TEST_VIEW</t>
+    <t>SAMPLE_VIEW, ADDITIONAL_TEST_VIEW, ADDITIONAL_TEST_DELETE, PATHOGEN_TEST_DELETE</t>
   </si>
   <si>
     <t>Export samples from SORMAS</t>
@@ -1127,7 +1127,7 @@
     <t>Able to create new contacts</t>
   </si>
   <si>
-    <t>PERSON_VIEW, CASE_VIEW, CONTACT_VIEW</t>
+    <t>CONTACT_VIEW, CASE_VIEW, PERSON_VIEW</t>
   </si>
   <si>
     <t>Edit existing contacts</t>
@@ -1136,7 +1136,7 @@
     <t>Able to edit existing contacts</t>
   </si>
   <si>
-    <t>PERSON_VIEW, CASE_VIEW, CONTACT_VIEW, PERSON_EDIT</t>
+    <t>CONTACT_VIEW, CASE_VIEW, PERSON_VIEW, PERSON_EDIT</t>
   </si>
   <si>
     <t>Archive contacts</t>
@@ -1151,7 +1151,7 @@
     <t>Able to delete contacts from the system</t>
   </si>
   <si>
-    <t>ADDITIONAL_TEST_DELETE, PATHOGEN_TEST_DELETE, TASK_VIEW, DOCUMENT_VIEW, SAMPLE_DELETE, PERSON_VIEW, DOCUMENT_DELETE, PERSON_DELETE, CASE_VIEW, TASK_DELETE, SAMPLE_VIEW, CONTACT_VIEW, ADDITIONAL_TEST_VIEW, VISIT_DELETE</t>
+    <t>SAMPLE_VIEW, ADDITIONAL_TEST_VIEW, DOCUMENT_VIEW, VISIT_DELETE, DOCUMENT_DELETE, CONTACT_VIEW, TASK_DELETE, TASK_VIEW, PERSON_VIEW, PERSON_DELETE, PATHOGEN_TEST_DELETE, CASE_VIEW, ADDITIONAL_TEST_DELETE, SAMPLE_DELETE</t>
   </si>
   <si>
     <t>Import contacts</t>
@@ -1172,7 +1172,7 @@
     <t>Able to create resulting cases from contacts</t>
   </si>
   <si>
-    <t>PERSON_VIEW, CONTACT_EDIT, CASE_CREATE, CASE_VIEW, CONTACT_VIEW, PERSON_EDIT</t>
+    <t>CONTACT_VIEW, CASE_VIEW, CONTACT_EDIT, CASE_CREATE, PERSON_VIEW, PERSON_EDIT</t>
   </si>
   <si>
     <t>Reassign the source case of contacts</t>
@@ -1181,7 +1181,7 @@
     <t>Able to reassign the source case of contacts</t>
   </si>
   <si>
-    <t>PERSON_VIEW, CONTACT_EDIT, CASE_VIEW, CONTACT_VIEW, PERSON_EDIT</t>
+    <t>CONTACT_VIEW, CASE_VIEW, CONTACT_EDIT, PERSON_VIEW, PERSON_EDIT</t>
   </si>
   <si>
     <t>Merge contacts</t>
@@ -1259,7 +1259,7 @@
     <t>Able to assign tasks to users</t>
   </si>
   <si>
-    <t>TASK_VIEW, TASK_EDIT</t>
+    <t>TASK_EDIT, TASK_VIEW</t>
   </si>
   <si>
     <t>Archive tasks</t>
@@ -1283,7 +1283,7 @@
     <t>Able to delete actions from the system</t>
   </si>
   <si>
-    <t>DOCUMENT_VIEW, DOCUMENT_DELETE, EVENT_VIEW</t>
+    <t>EVENT_VIEW, DOCUMENT_VIEW, DOCUMENT_DELETE</t>
   </si>
   <si>
     <t>Edit existing actions</t>
@@ -1322,7 +1322,7 @@
     <t>Able to delete events from the system</t>
   </si>
   <si>
-    <t>ADDITIONAL_TEST_DELETE, TASK_VIEW, PATHOGEN_TEST_DELETE, EVENTPARTICIPANT_DELETE, EVENT_VIEW, ACTION_DELETE, EVENTPARTICIPANT_VIEW, DOCUMENT_VIEW, SAMPLE_DELETE, PERSON_VIEW, DOCUMENT_DELETE, PERSON_DELETE, TASK_DELETE, SAMPLE_VIEW, ADDITIONAL_TEST_VIEW, VISIT_DELETE</t>
+    <t>EVENTPARTICIPANT_DELETE, SAMPLE_VIEW, ADDITIONAL_TEST_VIEW, EVENT_VIEW, DOCUMENT_VIEW, VISIT_DELETE, DOCUMENT_DELETE, TASK_DELETE, TASK_VIEW, PERSON_VIEW, PERSON_DELETE, PATHOGEN_TEST_DELETE, ACTION_DELETE, ADDITIONAL_TEST_DELETE, SAMPLE_DELETE, EVENTPARTICIPANT_VIEW</t>
   </si>
   <si>
     <t>Import events</t>
@@ -1340,7 +1340,7 @@
     <t>Can be responsible for an event</t>
   </si>
   <si>
-    <t>EVENT_EDIT, EVENT_VIEW</t>
+    <t>EVENT_VIEW, EVENT_EDIT</t>
   </si>
   <si>
     <t>View existing event participants</t>
@@ -1349,7 +1349,7 @@
     <t>Able to view existing event participants</t>
   </si>
   <si>
-    <t>PERSON_VIEW, EVENT_VIEW</t>
+    <t>EVENT_VIEW, PERSON_VIEW</t>
   </si>
   <si>
     <t>Create new event participants</t>
@@ -1358,7 +1358,7 @@
     <t>Able to create new event participants</t>
   </si>
   <si>
-    <t>PERSON_VIEW, EVENT_VIEW, EVENTPARTICIPANT_VIEW</t>
+    <t>EVENT_VIEW, EVENTPARTICIPANT_VIEW, PERSON_VIEW</t>
   </si>
   <si>
     <t>Edit existing event participants</t>
@@ -1367,7 +1367,7 @@
     <t>Able to edit existing event participants</t>
   </si>
   <si>
-    <t>PERSON_VIEW, EVENT_VIEW, EVENTPARTICIPANT_VIEW, PERSON_EDIT</t>
+    <t>EVENT_VIEW, EVENTPARTICIPANT_VIEW, PERSON_VIEW, PERSON_EDIT</t>
   </si>
   <si>
     <t>Event participant archive</t>
@@ -1382,7 +1382,7 @@
     <t>Able to delete event participants from the system</t>
   </si>
   <si>
-    <t>SAMPLE_DELETE, ADDITIONAL_TEST_DELETE, PERSON_VIEW, PATHOGEN_TEST_DELETE, PERSON_DELETE, SAMPLE_VIEW, EVENT_VIEW, ADDITIONAL_TEST_VIEW, EVENTPARTICIPANT_VIEW, VISIT_DELETE</t>
+    <t>SAMPLE_VIEW, ADDITIONAL_TEST_VIEW, EVENT_VIEW, VISIT_DELETE, ADDITIONAL_TEST_DELETE, SAMPLE_DELETE, EVENTPARTICIPANT_VIEW, PERSON_VIEW, PERSON_DELETE, PATHOGEN_TEST_DELETE</t>
   </si>
   <si>
     <t>Import event participants</t>
@@ -1397,7 +1397,7 @@
     <t>Able to create new event groups</t>
   </si>
   <si>
-    <t>EVENT_EDIT, EVENTGROUP_LINK, EVENT_VIEW</t>
+    <t>EVENT_VIEW, EVENTGROUP_LINK, EVENT_EDIT</t>
   </si>
   <si>
     <t>Edit existing event groups</t>
@@ -1535,7 +1535,7 @@
     <t>Able to view contact transmission chains on the dashboard</t>
   </si>
   <si>
-    <t>DASHBOARD_CONTACT_VIEW, PERSON_VIEW, CASE_VIEW, CONTACT_VIEW</t>
+    <t>DASHBOARD_CONTACT_VIEW, CONTACT_VIEW, CASE_VIEW, PERSON_VIEW</t>
   </si>
   <si>
     <t>Access campaigns dashboard</t>
@@ -1568,7 +1568,7 @@
     <t>Able to create new prescriptions</t>
   </si>
   <si>
-    <t>PERSON_VIEW, THERAPY_VIEW, CASE_VIEW</t>
+    <t>CASE_VIEW, THERAPY_VIEW, PERSON_VIEW</t>
   </si>
   <si>
     <t>Edit existing prescriptions</t>
@@ -1613,7 +1613,7 @@
     <t>Able to edit the clinical course of cases</t>
   </si>
   <si>
-    <t>PERSON_VIEW, THERAPY_VIEW, CASE_VIEW, CLINICAL_COURSE_VIEW</t>
+    <t>CLINICAL_COURSE_VIEW, CASE_VIEW, THERAPY_VIEW, PERSON_VIEW</t>
   </si>
   <si>
     <t>Create new clinical visits</t>
@@ -1649,7 +1649,7 @@
     <t>Able to edit existing port health info</t>
   </si>
   <si>
-    <t>PERSON_VIEW, PORT_HEALTH_INFO_VIEW, CASE_VIEW</t>
+    <t>CASE_VIEW, PORT_HEALTH_INFO_VIEW, PERSON_VIEW</t>
   </si>
   <si>
     <t>Aggregated Reporting</t>
@@ -1739,7 +1739,7 @@
     <t>Able to delete campaigns from the system</t>
   </si>
   <si>
-    <t>CAMPAIGN_VIEW, CAMPAIGN_FORM_DATA_VIEW, CAMPAIGN_FORM_DATA_DELETE</t>
+    <t>CAMPAIGN_VIEW, CAMPAIGN_FORM_DATA_DELETE, CAMPAIGN_FORM_DATA_VIEW</t>
   </si>
   <si>
     <t>View existing campaign form data</t>
@@ -1787,7 +1787,7 @@
     <t>Able to view existing travel entries</t>
   </si>
   <si>
-    <t>PERSON_VIEW, TRAVEL_ENTRY_MANAGEMENT_ACCESS</t>
+    <t>TRAVEL_ENTRY_MANAGEMENT_ACCESS, PERSON_VIEW</t>
   </si>
   <si>
     <t>Create new travel entries</t>
@@ -1796,7 +1796,7 @@
     <t>Able to create new travel entries</t>
   </si>
   <si>
-    <t>PERSON_VIEW, TRAVEL_ENTRY_VIEW, TRAVEL_ENTRY_MANAGEMENT_ACCESS</t>
+    <t>TRAVEL_ENTRY_VIEW, TRAVEL_ENTRY_MANAGEMENT_ACCESS, PERSON_VIEW</t>
   </si>
   <si>
     <t>Edit existing travel entries</t>
@@ -1805,7 +1805,7 @@
     <t>Able to edit existing travel entries</t>
   </si>
   <si>
-    <t>PERSON_VIEW, TRAVEL_ENTRY_VIEW, TRAVEL_ENTRY_MANAGEMENT_ACCESS, PERSON_EDIT</t>
+    <t>TRAVEL_ENTRY_VIEW, TRAVEL_ENTRY_MANAGEMENT_ACCESS, PERSON_VIEW, PERSON_EDIT</t>
   </si>
   <si>
     <t>Archive travel entries</t>
@@ -1820,7 +1820,7 @@
     <t>Able to delete travel entries from the system</t>
   </si>
   <si>
-    <t>DOCUMENT_VIEW, PERSON_VIEW, TRAVEL_ENTRY_VIEW, DOCUMENT_DELETE, TASK_VIEW, PERSON_DELETE, TASK_DELETE, TRAVEL_ENTRY_MANAGEMENT_ACCESS, VISIT_DELETE</t>
+    <t>TRAVEL_ENTRY_VIEW, DOCUMENT_VIEW, VISIT_DELETE, DOCUMENT_DELETE, TRAVEL_ENTRY_MANAGEMENT_ACCESS, TASK_DELETE, TASK_VIEW, PERSON_VIEW, PERSON_DELETE</t>
   </si>
   <si>
     <t>Environments</t>
@@ -1853,7 +1853,7 @@
     <t>Able to delete environments from the system</t>
   </si>
   <si>
-    <t>ENVIRONMENT_VIEW, ENVIRONMENT_PATHOGEN_TEST_DELETE, ENVIRONMENT_SAMPLE_DELETE, ENVIRONMENT_SAMPLE_VIEW</t>
+    <t>ENVIRONMENT_SAMPLE_DELETE, ENVIRONMENT_SAMPLE_VIEW, ENVIRONMENT_VIEW, ENVIRONMENT_PATHOGEN_TEST_DELETE</t>
   </si>
   <si>
     <t>Import environments</t>
@@ -1862,7 +1862,7 @@
     <t>Able to import environments</t>
   </si>
   <si>
-    <t>ENVIRONMENT_VIEW, ENVIRONMENT_CREATE</t>
+    <t>ENVIRONMENT_CREATE, ENVIRONMENT_VIEW</t>
   </si>
   <si>
     <t>Export environments</t>
@@ -1895,7 +1895,7 @@
     <t>Able to edit environment samples dispatch information</t>
   </si>
   <si>
-    <t>ENVIRONMENT_SAMPLE_EDIT, ENVIRONMENT_SAMPLE_VIEW</t>
+    <t>ENVIRONMENT_SAMPLE_VIEW, ENVIRONMENT_SAMPLE_EDIT</t>
   </si>
   <si>
     <t>Edit environment samples receival information</t>
@@ -1910,7 +1910,7 @@
     <t>Able to delete environment samples from the system</t>
   </si>
   <si>
-    <t>ENVIRONMENT_PATHOGEN_TEST_DELETE, ENVIRONMENT_SAMPLE_VIEW</t>
+    <t>ENVIRONMENT_SAMPLE_VIEW, ENVIRONMENT_PATHOGEN_TEST_DELETE</t>
   </si>
   <si>
     <t>Import environment samples</t>
@@ -2081,7 +2081,7 @@
     <t>Able to work with messages</t>
   </si>
   <si>
-    <t>PATHOGEN_TEST_DELETE, PATHOGEN_TEST_EDIT, IMMUNIZATION_DELETE, IMMUNIZATION_EDIT, IMMUNIZATION_CREATE, PERSON_VIEW, PATHOGEN_TEST_CREATE, IMMUNIZATION_VIEW, PERSON_DELETE, SAMPLE_VIEW, SAMPLE_CREATE, EXTERNAL_MESSAGE_VIEW, SAMPLE_EDIT, VISIT_DELETE, PERSON_EDIT</t>
+    <t>SAMPLE_VIEW, VISIT_DELETE, SAMPLE_EDIT, PATHOGEN_TEST_EDIT, IMMUNIZATION_VIEW, EXTERNAL_MESSAGE_VIEW, IMMUNIZATION_DELETE, PERSON_VIEW, PATHOGEN_TEST_DELETE, PERSON_EDIT, PERSON_DELETE, SAMPLE_CREATE, PATHOGEN_TEST_CREATE, IMMUNIZATION_EDIT, IMMUNIZATION_CREATE</t>
   </si>
   <si>
     <t>Push external messages to the system</t>
@@ -2276,7 +2276,7 @@
     <t>SORMAS Version</t>
   </si>
   <si>
-    <t>1.95.0-SNAPSHOT</t>
+    <t>1.0.0</t>
   </si>
 </sst>
 </file>

</xml_diff>